<commit_message>
Add eLife COD coding
</commit_message>
<xml_diff>
--- a/USA/state/data/cod/GHE cause_list_icd_codes_updated10August2016_elife.xlsx
+++ b/USA/state/data/cod/GHE cause_list_icd_codes_updated10August2016_elife.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5293,7 +5293,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5327,6 +5327,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5494,7 +5500,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="209">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5838,20 +5844,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="15" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -5972,40 +5969,137 @@
     <xf numFmtId="49" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="7" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="7" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="7" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="1" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6287,10 +6381,14 @@
   <dimension ref="A1:R185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:H3"/>
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="11" max="11" width="10.83203125" style="202"/>
+    <col min="14" max="14" width="10.83203125" style="202"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="79" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
@@ -6300,20 +6398,20 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="167" t="s">
+      <c r="D1" s="172" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="168"/>
-      <c r="F1" s="168"/>
-      <c r="G1" s="168"/>
-      <c r="H1" s="168"/>
+      <c r="E1" s="173"/>
+      <c r="F1" s="173"/>
+      <c r="G1" s="173"/>
+      <c r="H1" s="173"/>
       <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="177" t="s">
         <v>5</v>
       </c>
       <c r="L1" s="5" t="s">
@@ -6322,7 +6420,7 @@
       <c r="M1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="177" t="s">
         <v>8</v>
       </c>
       <c r="O1" s="5" t="s">
@@ -6357,62 +6455,62 @@
       <c r="H2" s="12"/>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
-      <c r="K2" s="14"/>
+      <c r="K2" s="178"/>
       <c r="L2" s="14"/>
       <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="N2" s="178"/>
       <c r="O2" s="14"/>
       <c r="P2" s="15"/>
       <c r="Q2" s="16"/>
       <c r="R2" s="17"/>
     </row>
-    <row r="3" spans="1:18" s="178" customFormat="1" ht="182" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" s="171" customFormat="1" ht="182" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="169" t="s">
+      <c r="C3" s="164" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="170" t="s">
+      <c r="D3" s="165" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="171" t="s">
+      <c r="E3" s="174" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="172"/>
-      <c r="G3" s="172"/>
-      <c r="H3" s="172"/>
-      <c r="I3" s="173" t="s">
+      <c r="F3" s="175"/>
+      <c r="G3" s="175"/>
+      <c r="H3" s="175"/>
+      <c r="I3" s="166" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="173" t="s">
+      <c r="J3" s="166" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="174" t="s">
+      <c r="K3" s="179" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="174" t="s">
+      <c r="L3" s="167" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="175" t="s">
+      <c r="M3" s="168" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="174" t="s">
+      <c r="N3" s="179" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="174" t="s">
+      <c r="O3" s="167" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="176" t="s">
+      <c r="P3" s="169" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="176" t="s">
+      <c r="Q3" s="169" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="177" t="s">
+      <c r="R3" s="170" t="s">
         <v>31</v>
       </c>
     </row>
@@ -6441,7 +6539,7 @@
       <c r="J4" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="180" t="s">
         <v>39</v>
       </c>
       <c r="L4" s="28" t="s">
@@ -6450,7 +6548,7 @@
       <c r="M4" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="28" t="s">
+      <c r="N4" s="180" t="s">
         <v>42</v>
       </c>
       <c r="O4" s="28" t="s">
@@ -6491,7 +6589,7 @@
       <c r="J5" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="K5" s="39" t="s">
+      <c r="K5" s="181" t="s">
         <v>53</v>
       </c>
       <c r="L5" s="39" t="s">
@@ -6500,7 +6598,7 @@
       <c r="M5" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="N5" s="39" t="s">
+      <c r="N5" s="181" t="s">
         <v>55</v>
       </c>
       <c r="O5" s="39" t="s">
@@ -6541,7 +6639,7 @@
       <c r="J6" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="K6" s="39" t="s">
+      <c r="K6" s="181" t="s">
         <v>66</v>
       </c>
       <c r="L6" s="39" t="s">
@@ -6550,7 +6648,7 @@
       <c r="M6" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="N6" s="39" t="s">
+      <c r="N6" s="181" t="s">
         <v>68</v>
       </c>
       <c r="O6" s="39" t="s">
@@ -6591,7 +6689,7 @@
       <c r="J7" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="49" t="s">
+      <c r="K7" s="181" t="s">
         <v>77</v>
       </c>
       <c r="L7" s="49" t="s">
@@ -6600,7 +6698,7 @@
       <c r="M7" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="N7" s="49" t="s">
+      <c r="N7" s="181" t="s">
         <v>79</v>
       </c>
       <c r="O7" s="49" t="s">
@@ -6641,7 +6739,7 @@
       <c r="J8" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K8" s="50" t="s">
+      <c r="K8" s="182" t="s">
         <v>69</v>
       </c>
       <c r="L8" s="50" t="s">
@@ -6650,7 +6748,7 @@
       <c r="M8" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N8" s="49" t="s">
+      <c r="N8" s="181" t="s">
         <v>86</v>
       </c>
       <c r="O8" s="49" t="s">
@@ -6691,7 +6789,7 @@
       <c r="J9" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="K9" s="51" t="s">
+      <c r="K9" s="183" t="s">
         <v>94</v>
       </c>
       <c r="L9" s="51" t="s">
@@ -6700,7 +6798,7 @@
       <c r="M9" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="N9" s="49" t="s">
+      <c r="N9" s="181" t="s">
         <v>96</v>
       </c>
       <c r="O9" s="49" t="s">
@@ -6739,7 +6837,7 @@
       <c r="J10" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="K10" s="54" t="s">
+      <c r="K10" s="184" t="s">
         <v>101</v>
       </c>
       <c r="L10" s="54" t="s">
@@ -6748,7 +6846,7 @@
       <c r="M10" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="N10" s="54" t="s">
+      <c r="N10" s="184" t="s">
         <v>103</v>
       </c>
       <c r="O10" s="54" t="s">
@@ -6789,7 +6887,7 @@
       <c r="J11" s="38">
         <v>137</v>
       </c>
-      <c r="K11" s="39" t="s">
+      <c r="K11" s="181" t="s">
         <v>109</v>
       </c>
       <c r="L11" s="39" t="s">
@@ -6798,7 +6896,7 @@
       <c r="M11" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="N11" s="39" t="s">
+      <c r="N11" s="181" t="s">
         <v>112</v>
       </c>
       <c r="O11" s="39" t="s">
@@ -6839,7 +6937,7 @@
       <c r="J12" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="K12" s="39" t="s">
+      <c r="K12" s="181" t="s">
         <v>121</v>
       </c>
       <c r="L12" s="39" t="s">
@@ -6848,7 +6946,7 @@
       <c r="M12" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="N12" s="55" t="s">
+      <c r="N12" s="200" t="s">
         <v>123</v>
       </c>
       <c r="O12" s="55" t="s">
@@ -6889,7 +6987,7 @@
       <c r="J13" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="K13" s="40" t="s">
+      <c r="K13" s="183" t="s">
         <v>134</v>
       </c>
       <c r="L13" s="40" t="s">
@@ -6898,7 +6996,7 @@
       <c r="M13" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="N13" s="39" t="s">
+      <c r="N13" s="181" t="s">
         <v>137</v>
       </c>
       <c r="O13" s="39" t="s">
@@ -6939,7 +7037,7 @@
       <c r="J14" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="K14" s="51" t="s">
+      <c r="K14" s="183" t="s">
         <v>147</v>
       </c>
       <c r="L14" s="51" t="s">
@@ -6948,7 +7046,7 @@
       <c r="M14" s="51" t="s">
         <v>148</v>
       </c>
-      <c r="N14" s="49" t="s">
+      <c r="N14" s="181" t="s">
         <v>149</v>
       </c>
       <c r="O14" s="49" t="s">
@@ -6989,7 +7087,7 @@
       <c r="J15" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="K15" s="51" t="s">
+      <c r="K15" s="183" t="s">
         <v>158</v>
       </c>
       <c r="L15" s="51" t="s">
@@ -6998,7 +7096,7 @@
       <c r="M15" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="N15" s="49" t="s">
+      <c r="N15" s="181" t="s">
         <v>160</v>
       </c>
       <c r="O15" s="49" t="s">
@@ -7039,7 +7137,7 @@
       <c r="J16" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="K16" s="51" t="s">
+      <c r="K16" s="183" t="s">
         <v>168</v>
       </c>
       <c r="L16" s="51" t="s">
@@ -7048,7 +7146,7 @@
       <c r="M16" s="51" t="s">
         <v>169</v>
       </c>
-      <c r="N16" s="49" t="s">
+      <c r="N16" s="181" t="s">
         <v>170</v>
       </c>
       <c r="O16" s="49" t="s">
@@ -7089,7 +7187,7 @@
       <c r="J17" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="K17" s="51" t="s">
+      <c r="K17" s="183" t="s">
         <v>178</v>
       </c>
       <c r="L17" s="51" t="s">
@@ -7098,7 +7196,7 @@
       <c r="M17" s="51" t="s">
         <v>179</v>
       </c>
-      <c r="N17" s="49" t="s">
+      <c r="N17" s="181" t="s">
         <v>180</v>
       </c>
       <c r="O17" s="49" t="s">
@@ -7139,7 +7237,7 @@
       <c r="J18" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="K18" s="51" t="s">
+      <c r="K18" s="183" t="s">
         <v>190</v>
       </c>
       <c r="L18" s="51" t="s">
@@ -7148,7 +7246,7 @@
       <c r="M18" s="57" t="s">
         <v>192</v>
       </c>
-      <c r="N18" s="49" t="s">
+      <c r="N18" s="181" t="s">
         <v>193</v>
       </c>
       <c r="O18" s="49" t="s">
@@ -7189,7 +7287,7 @@
       <c r="J19" s="38" t="s">
         <v>203</v>
       </c>
-      <c r="K19" s="39" t="s">
+      <c r="K19" s="181" t="s">
         <v>204</v>
       </c>
       <c r="L19" s="39" t="s">
@@ -7198,7 +7296,7 @@
       <c r="M19" s="40" t="s">
         <v>205</v>
       </c>
-      <c r="N19" s="58" t="s">
+      <c r="N19" s="180" t="s">
         <v>206</v>
       </c>
       <c r="O19" s="58" t="s">
@@ -7239,7 +7337,7 @@
       <c r="J20" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="K20" s="39" t="s">
+      <c r="K20" s="181" t="s">
         <v>217</v>
       </c>
       <c r="L20" s="40" t="s">
@@ -7248,7 +7346,7 @@
       <c r="M20" s="39" t="s">
         <v>219</v>
       </c>
-      <c r="N20" s="58" t="s">
+      <c r="N20" s="180" t="s">
         <v>220</v>
       </c>
       <c r="O20" s="58" t="s">
@@ -7285,7 +7383,7 @@
       <c r="J21" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="K21" s="38" t="s">
+      <c r="K21" s="185" t="s">
         <v>69</v>
       </c>
       <c r="L21" s="38" t="s">
@@ -7294,7 +7392,7 @@
       <c r="M21" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="N21" s="38" t="s">
+      <c r="N21" s="185" t="s">
         <v>227</v>
       </c>
       <c r="O21" s="38" t="s">
@@ -7335,7 +7433,7 @@
       <c r="J22" s="38" t="s">
         <v>234</v>
       </c>
-      <c r="K22" s="40" t="s">
+      <c r="K22" s="183" t="s">
         <v>235</v>
       </c>
       <c r="L22" s="40" t="s">
@@ -7344,7 +7442,7 @@
       <c r="M22" s="40" t="s">
         <v>236</v>
       </c>
-      <c r="N22" s="39" t="s">
+      <c r="N22" s="181" t="s">
         <v>237</v>
       </c>
       <c r="O22" s="39" t="s">
@@ -7385,7 +7483,7 @@
       <c r="J23" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="K23" s="40" t="s">
+      <c r="K23" s="183" t="s">
         <v>247</v>
       </c>
       <c r="L23" s="40" t="s">
@@ -7394,7 +7492,7 @@
       <c r="M23" s="40" t="s">
         <v>249</v>
       </c>
-      <c r="N23" s="39" t="s">
+      <c r="N23" s="181" t="s">
         <v>250</v>
       </c>
       <c r="O23" s="39" t="s">
@@ -7435,13 +7533,13 @@
       <c r="J24" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="K24" s="51" t="s">
+      <c r="K24" s="183" t="s">
         <v>256</v>
       </c>
       <c r="L24" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="N24" s="49" t="s">
+      <c r="N24" s="181" t="s">
         <v>257</v>
       </c>
       <c r="O24" s="49" t="s">
@@ -7482,7 +7580,7 @@
       <c r="J25" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K25" s="51" t="s">
+      <c r="K25" s="183" t="s">
         <v>262</v>
       </c>
       <c r="L25" s="51" t="s">
@@ -7491,7 +7589,7 @@
       <c r="M25" s="59" t="s">
         <v>264</v>
       </c>
-      <c r="N25" s="49" t="s">
+      <c r="N25" s="181" t="s">
         <v>265</v>
       </c>
       <c r="O25" s="49" t="s">
@@ -7532,7 +7630,7 @@
       <c r="J26" s="27" t="s">
         <v>270</v>
       </c>
-      <c r="K26" s="49">
+      <c r="K26" s="181">
         <v>120</v>
       </c>
       <c r="L26" s="49">
@@ -7541,7 +7639,7 @@
       <c r="M26" s="51" t="s">
         <v>271</v>
       </c>
-      <c r="N26" s="49" t="s">
+      <c r="N26" s="181" t="s">
         <v>272</v>
       </c>
       <c r="O26" s="49" t="s">
@@ -7582,7 +7680,7 @@
       <c r="J27" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K27" s="51" t="s">
+      <c r="K27" s="183" t="s">
         <v>279</v>
       </c>
       <c r="L27" s="51" t="s">
@@ -7591,7 +7689,7 @@
       <c r="M27" s="51" t="s">
         <v>280</v>
       </c>
-      <c r="N27" s="49" t="s">
+      <c r="N27" s="181" t="s">
         <v>281</v>
       </c>
       <c r="O27" s="49" t="s">
@@ -7632,7 +7730,7 @@
       <c r="J28" s="27" t="s">
         <v>288</v>
       </c>
-      <c r="K28" s="49" t="s">
+      <c r="K28" s="181" t="s">
         <v>289</v>
       </c>
       <c r="L28" s="49">
@@ -7641,7 +7739,7 @@
       <c r="M28" s="49" t="s">
         <v>290</v>
       </c>
-      <c r="N28" s="49" t="s">
+      <c r="N28" s="181" t="s">
         <v>291</v>
       </c>
       <c r="O28" s="50" t="s">
@@ -7682,7 +7780,7 @@
       <c r="J29" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K29" s="49">
+      <c r="K29" s="181">
         <v>125.3</v>
       </c>
       <c r="L29" s="49" t="s">
@@ -7691,7 +7789,7 @@
       <c r="M29" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N29" s="49" t="s">
+      <c r="N29" s="181" t="s">
         <v>297</v>
       </c>
       <c r="O29" s="49" t="s">
@@ -7732,7 +7830,7 @@
       <c r="J30" s="38" t="s">
         <v>303</v>
       </c>
-      <c r="K30" s="40" t="s">
+      <c r="K30" s="183" t="s">
         <v>304</v>
       </c>
       <c r="L30" s="40" t="s">
@@ -7741,7 +7839,7 @@
       <c r="M30" s="40" t="s">
         <v>305</v>
       </c>
-      <c r="N30" s="39" t="s">
+      <c r="N30" s="181" t="s">
         <v>306</v>
       </c>
       <c r="O30" s="39" t="s">
@@ -7782,7 +7880,7 @@
       <c r="J31" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="K31" s="40" t="s">
+      <c r="K31" s="183" t="s">
         <v>312</v>
       </c>
       <c r="L31" s="40" t="s">
@@ -7791,7 +7889,7 @@
       <c r="M31" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="N31" s="39" t="s">
+      <c r="N31" s="181" t="s">
         <v>313</v>
       </c>
       <c r="O31" s="39" t="s">
@@ -7832,7 +7930,7 @@
       <c r="J32" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="K32" s="40" t="s">
+      <c r="K32" s="183" t="s">
         <v>319</v>
       </c>
       <c r="L32" s="39" t="s">
@@ -7841,7 +7939,7 @@
       <c r="M32" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="N32" s="39" t="s">
+      <c r="N32" s="181" t="s">
         <v>320</v>
       </c>
       <c r="O32" s="41" t="s">
@@ -7882,7 +7980,7 @@
       <c r="J33" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="K33" s="40" t="s">
+      <c r="K33" s="183" t="s">
         <v>327</v>
       </c>
       <c r="L33" s="40" t="s">
@@ -7891,7 +7989,7 @@
       <c r="M33" s="40" t="s">
         <v>328</v>
       </c>
-      <c r="N33" s="39" t="s">
+      <c r="N33" s="181" t="s">
         <v>329</v>
       </c>
       <c r="O33" s="39" t="s">
@@ -7932,7 +8030,7 @@
       <c r="J34" s="38" t="s">
         <v>336</v>
       </c>
-      <c r="K34" s="39" t="s">
+      <c r="K34" s="181" t="s">
         <v>337</v>
       </c>
       <c r="L34" s="39" t="s">
@@ -7941,7 +8039,7 @@
       <c r="M34" s="39" t="s">
         <v>338</v>
       </c>
-      <c r="N34" s="55" t="s">
+      <c r="N34" s="200" t="s">
         <v>339</v>
       </c>
       <c r="O34" s="55" t="s">
@@ -7982,7 +8080,7 @@
       <c r="J35" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K35" s="51" t="s">
+      <c r="K35" s="183" t="s">
         <v>344</v>
       </c>
       <c r="L35" s="51">
@@ -7991,7 +8089,7 @@
       <c r="M35" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N35" s="49" t="s">
+      <c r="N35" s="181" t="s">
         <v>345</v>
       </c>
       <c r="O35" s="49" t="s">
@@ -8032,7 +8130,7 @@
       <c r="J36" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K36" s="51" t="s">
+      <c r="K36" s="183" t="s">
         <v>350</v>
       </c>
       <c r="L36" s="49" t="s">
@@ -8041,7 +8139,7 @@
       <c r="M36" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N36" s="49" t="s">
+      <c r="N36" s="181" t="s">
         <v>351</v>
       </c>
       <c r="O36" s="49" t="s">
@@ -8082,7 +8180,7 @@
       <c r="J37" s="27" t="s">
         <v>356</v>
       </c>
-      <c r="K37" s="49">
+      <c r="K37" s="181">
         <v>126</v>
       </c>
       <c r="L37" s="49">
@@ -8091,7 +8189,7 @@
       <c r="M37" s="49" t="s">
         <v>357</v>
       </c>
-      <c r="N37" s="49" t="s">
+      <c r="N37" s="181" t="s">
         <v>358</v>
       </c>
       <c r="O37" s="49" t="s">
@@ -8128,7 +8226,7 @@
       <c r="J38" s="53" t="s">
         <v>362</v>
       </c>
-      <c r="K38" s="54" t="s">
+      <c r="K38" s="184" t="s">
         <v>363</v>
       </c>
       <c r="L38" s="54" t="s">
@@ -8137,7 +8235,7 @@
       <c r="M38" s="54" t="s">
         <v>365</v>
       </c>
-      <c r="N38" s="54" t="s">
+      <c r="N38" s="184" t="s">
         <v>366</v>
       </c>
       <c r="O38" s="54" t="s">
@@ -8174,7 +8272,7 @@
       <c r="J39" s="53" t="s">
         <v>371</v>
       </c>
-      <c r="K39" s="54" t="s">
+      <c r="K39" s="184" t="s">
         <v>372</v>
       </c>
       <c r="L39" s="54" t="s">
@@ -8183,7 +8281,7 @@
       <c r="M39" s="54" t="s">
         <v>374</v>
       </c>
-      <c r="N39" s="54" t="s">
+      <c r="N39" s="184" t="s">
         <v>375</v>
       </c>
       <c r="O39" s="54" t="s">
@@ -8199,53 +8297,53 @@
         <v>379</v>
       </c>
     </row>
-    <row r="40" spans="1:18" s="163" customFormat="1" ht="39" x14ac:dyDescent="0.2">
-      <c r="A40" s="153" t="s">
+    <row r="40" spans="1:18" s="160" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A40" s="150" t="s">
         <v>380</v>
       </c>
-      <c r="B40" s="154" t="s">
+      <c r="B40" s="151" t="s">
         <v>381</v>
       </c>
-      <c r="C40" s="155" t="s">
+      <c r="C40" s="152" t="s">
         <v>382</v>
       </c>
-      <c r="D40" s="156"/>
-      <c r="E40" s="157" t="s">
+      <c r="D40" s="153"/>
+      <c r="E40" s="154" t="s">
         <v>383</v>
       </c>
-      <c r="F40" s="158" t="s">
+      <c r="F40" s="155" t="s">
         <v>384</v>
       </c>
-      <c r="G40" s="159"/>
-      <c r="H40" s="159"/>
-      <c r="I40" s="160" t="s">
+      <c r="G40" s="156"/>
+      <c r="H40" s="156"/>
+      <c r="I40" s="157" t="s">
         <v>385</v>
       </c>
-      <c r="J40" s="160" t="s">
+      <c r="J40" s="157" t="s">
         <v>386</v>
       </c>
-      <c r="K40" s="161" t="s">
+      <c r="K40" s="181" t="s">
         <v>387</v>
       </c>
-      <c r="L40" s="161" t="s">
+      <c r="L40" s="158" t="s">
         <v>387</v>
       </c>
-      <c r="M40" s="161" t="s">
+      <c r="M40" s="158" t="s">
         <v>388</v>
       </c>
-      <c r="N40" s="161" t="s">
+      <c r="N40" s="181" t="s">
         <v>389</v>
       </c>
-      <c r="O40" s="161" t="s">
+      <c r="O40" s="158" t="s">
         <v>389</v>
       </c>
-      <c r="P40" s="162" t="s">
+      <c r="P40" s="159" t="s">
         <v>390</v>
       </c>
-      <c r="Q40" s="162" t="s">
+      <c r="Q40" s="159" t="s">
         <v>391</v>
       </c>
-      <c r="R40" s="162" t="s">
+      <c r="R40" s="159" t="s">
         <v>69</v>
       </c>
     </row>
@@ -8274,7 +8372,7 @@
       <c r="J41" s="27" t="s">
         <v>397</v>
       </c>
-      <c r="K41" s="49" t="s">
+      <c r="K41" s="181" t="s">
         <v>398</v>
       </c>
       <c r="L41" s="49" t="s">
@@ -8283,7 +8381,7 @@
       <c r="M41" s="49" t="s">
         <v>399</v>
       </c>
-      <c r="N41" s="49" t="s">
+      <c r="N41" s="181" t="s">
         <v>400</v>
       </c>
       <c r="O41" s="49" t="s">
@@ -8324,7 +8422,7 @@
       <c r="J42" s="27" t="s">
         <v>408</v>
       </c>
-      <c r="K42" s="49" t="s">
+      <c r="K42" s="181" t="s">
         <v>409</v>
       </c>
       <c r="L42" s="49" t="s">
@@ -8333,7 +8431,7 @@
       <c r="M42" s="49" t="s">
         <v>410</v>
       </c>
-      <c r="N42" s="49" t="s">
+      <c r="N42" s="181" t="s">
         <v>411</v>
       </c>
       <c r="O42" s="49" t="s">
@@ -8374,7 +8472,7 @@
       <c r="J43" s="27" t="s">
         <v>418</v>
       </c>
-      <c r="K43" s="49" t="s">
+      <c r="K43" s="181" t="s">
         <v>419</v>
       </c>
       <c r="L43" s="49" t="s">
@@ -8383,7 +8481,7 @@
       <c r="M43" s="49" t="s">
         <v>420</v>
       </c>
-      <c r="N43" s="49" t="s">
+      <c r="N43" s="181" t="s">
         <v>421</v>
       </c>
       <c r="O43" s="49" t="s">
@@ -8399,53 +8497,53 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:18" s="163" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="153" t="s">
+    <row r="44" spans="1:18" s="160" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="150" t="s">
         <v>422</v>
       </c>
-      <c r="B44" s="154" t="s">
+      <c r="B44" s="151" t="s">
         <v>423</v>
       </c>
-      <c r="C44" s="155" t="s">
+      <c r="C44" s="152" t="s">
         <v>424</v>
       </c>
-      <c r="D44" s="156"/>
-      <c r="E44" s="157" t="s">
+      <c r="D44" s="153"/>
+      <c r="E44" s="154" t="s">
         <v>425</v>
       </c>
-      <c r="F44" s="158" t="s">
+      <c r="F44" s="155" t="s">
         <v>426</v>
       </c>
-      <c r="G44" s="159"/>
-      <c r="H44" s="159"/>
-      <c r="I44" s="160" t="s">
+      <c r="G44" s="156"/>
+      <c r="H44" s="156"/>
+      <c r="I44" s="157" t="s">
         <v>427</v>
       </c>
-      <c r="J44" s="160" t="s">
+      <c r="J44" s="157" t="s">
         <v>428</v>
       </c>
-      <c r="K44" s="161" t="s">
+      <c r="K44" s="181" t="s">
         <v>429</v>
       </c>
-      <c r="L44" s="161" t="s">
+      <c r="L44" s="158" t="s">
         <v>429</v>
       </c>
-      <c r="M44" s="161" t="s">
+      <c r="M44" s="158" t="s">
         <v>430</v>
       </c>
-      <c r="N44" s="161" t="s">
+      <c r="N44" s="181" t="s">
         <v>431</v>
       </c>
-      <c r="O44" s="161" t="s">
+      <c r="O44" s="158" t="s">
         <v>431</v>
       </c>
-      <c r="P44" s="162" t="s">
+      <c r="P44" s="159" t="s">
         <v>432</v>
       </c>
-      <c r="Q44" s="162" t="s">
+      <c r="Q44" s="159" t="s">
         <v>433</v>
       </c>
-      <c r="R44" s="166" t="s">
+      <c r="R44" s="163" t="s">
         <v>434</v>
       </c>
     </row>
@@ -8474,7 +8572,7 @@
       <c r="J45" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="K45" s="51" t="s">
+      <c r="K45" s="183" t="s">
         <v>441</v>
       </c>
       <c r="L45" s="51" t="s">
@@ -8483,7 +8581,7 @@
       <c r="M45" s="49" t="s">
         <v>442</v>
       </c>
-      <c r="N45" s="49" t="s">
+      <c r="N45" s="181" t="s">
         <v>443</v>
       </c>
       <c r="O45" s="49" t="s">
@@ -8524,7 +8622,7 @@
       <c r="J46" s="27" t="s">
         <v>450</v>
       </c>
-      <c r="K46" s="49">
+      <c r="K46" s="181">
         <v>670</v>
       </c>
       <c r="L46" s="49">
@@ -8533,7 +8631,7 @@
       <c r="M46" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N46" s="49" t="s">
+      <c r="N46" s="181" t="s">
         <v>451</v>
       </c>
       <c r="O46" s="49" t="s">
@@ -8574,7 +8672,7 @@
       <c r="J47" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K47" s="49">
+      <c r="K47" s="181">
         <v>642</v>
       </c>
       <c r="L47" s="49">
@@ -8583,7 +8681,7 @@
       <c r="M47" s="27" t="s">
         <v>457</v>
       </c>
-      <c r="N47" s="49" t="s">
+      <c r="N47" s="181" t="s">
         <v>458</v>
       </c>
       <c r="O47" s="49" t="s">
@@ -8624,7 +8722,7 @@
       <c r="J48" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K48" s="49">
+      <c r="K48" s="181">
         <v>660</v>
       </c>
       <c r="L48" s="49">
@@ -8633,7 +8731,7 @@
       <c r="M48" s="49" t="s">
         <v>463</v>
       </c>
-      <c r="N48" s="49" t="s">
+      <c r="N48" s="181" t="s">
         <v>464</v>
       </c>
       <c r="O48" s="49" t="s">
@@ -8674,7 +8772,7 @@
       <c r="J49" s="27" t="s">
         <v>470</v>
       </c>
-      <c r="K49" s="49" t="s">
+      <c r="K49" s="181" t="s">
         <v>471</v>
       </c>
       <c r="L49" s="49" t="s">
@@ -8683,7 +8781,7 @@
       <c r="M49" s="49" t="s">
         <v>472</v>
       </c>
-      <c r="N49" s="49" t="s">
+      <c r="N49" s="181" t="s">
         <v>473</v>
       </c>
       <c r="O49" s="49" t="s">
@@ -8720,7 +8818,7 @@
       <c r="J50" s="53" t="s">
         <v>480</v>
       </c>
-      <c r="K50" s="54" t="s">
+      <c r="K50" s="184" t="s">
         <v>481</v>
       </c>
       <c r="L50" s="54" t="s">
@@ -8729,7 +8827,7 @@
       <c r="M50" s="54" t="s">
         <v>482</v>
       </c>
-      <c r="N50" s="54" t="s">
+      <c r="N50" s="184" t="s">
         <v>483</v>
       </c>
       <c r="O50" s="54" t="s">
@@ -8745,53 +8843,53 @@
         <v>486</v>
       </c>
     </row>
-    <row r="51" spans="1:18" s="163" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="A51" s="153" t="s">
+    <row r="51" spans="1:18" s="160" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A51" s="150" t="s">
         <v>487</v>
       </c>
-      <c r="B51" s="154" t="s">
+      <c r="B51" s="151" t="s">
         <v>488</v>
       </c>
-      <c r="C51" s="155" t="s">
+      <c r="C51" s="152" t="s">
         <v>489</v>
       </c>
-      <c r="D51" s="156"/>
-      <c r="E51" s="157" t="s">
+      <c r="D51" s="153"/>
+      <c r="E51" s="154" t="s">
         <v>490</v>
       </c>
-      <c r="F51" s="158" t="s">
+      <c r="F51" s="155" t="s">
         <v>491</v>
       </c>
-      <c r="G51" s="159"/>
-      <c r="H51" s="159"/>
-      <c r="I51" s="160" t="s">
+      <c r="G51" s="156"/>
+      <c r="H51" s="156"/>
+      <c r="I51" s="157" t="s">
         <v>492</v>
       </c>
-      <c r="J51" s="160" t="s">
+      <c r="J51" s="157" t="s">
         <v>493</v>
       </c>
-      <c r="K51" s="161" t="s">
+      <c r="K51" s="181" t="s">
         <v>494</v>
       </c>
-      <c r="L51" s="161" t="s">
+      <c r="L51" s="158" t="s">
         <v>495</v>
       </c>
-      <c r="M51" s="161" t="s">
+      <c r="M51" s="158" t="s">
         <v>496</v>
       </c>
-      <c r="N51" s="161" t="s">
+      <c r="N51" s="181" t="s">
         <v>497</v>
       </c>
-      <c r="O51" s="161" t="s">
+      <c r="O51" s="158" t="s">
         <v>497</v>
       </c>
-      <c r="P51" s="162" t="s">
+      <c r="P51" s="159" t="s">
         <v>496</v>
       </c>
-      <c r="Q51" s="162" t="s">
+      <c r="Q51" s="159" t="s">
         <v>498</v>
       </c>
-      <c r="R51" s="166" t="s">
+      <c r="R51" s="163" t="s">
         <v>499</v>
       </c>
     </row>
@@ -8820,7 +8918,7 @@
       <c r="J52" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K52" s="49" t="s">
+      <c r="K52" s="181" t="s">
         <v>504</v>
       </c>
       <c r="L52" s="49" t="s">
@@ -8829,7 +8927,7 @@
       <c r="M52" s="54" t="s">
         <v>505</v>
       </c>
-      <c r="N52" s="49" t="s">
+      <c r="N52" s="181" t="s">
         <v>506</v>
       </c>
       <c r="O52" s="49" t="s">
@@ -8870,7 +8968,7 @@
       <c r="J53" s="27" t="s">
         <v>513</v>
       </c>
-      <c r="K53" s="49" t="s">
+      <c r="K53" s="181" t="s">
         <v>514</v>
       </c>
       <c r="L53" s="49" t="s">
@@ -8879,7 +8977,7 @@
       <c r="M53" s="49" t="s">
         <v>515</v>
       </c>
-      <c r="N53" s="49" t="s">
+      <c r="N53" s="181" t="s">
         <v>516</v>
       </c>
       <c r="O53" s="49" t="s">
@@ -8916,7 +9014,7 @@
       <c r="J54" s="53" t="s">
         <v>523</v>
       </c>
-      <c r="K54" s="54" t="s">
+      <c r="K54" s="184" t="s">
         <v>524</v>
       </c>
       <c r="L54" s="54" t="s">
@@ -8925,7 +9023,7 @@
       <c r="M54" s="54" t="s">
         <v>526</v>
       </c>
-      <c r="N54" s="54" t="s">
+      <c r="N54" s="184" t="s">
         <v>527</v>
       </c>
       <c r="O54" s="54" t="s">
@@ -8966,7 +9064,7 @@
       <c r="J55" s="27" t="s">
         <v>536</v>
       </c>
-      <c r="K55" s="78" t="s">
+      <c r="K55" s="186" t="s">
         <v>537</v>
       </c>
       <c r="L55" s="78" t="s">
@@ -8975,7 +9073,7 @@
       <c r="M55" s="49" t="s">
         <v>539</v>
       </c>
-      <c r="N55" s="78" t="s">
+      <c r="N55" s="186" t="s">
         <v>540</v>
       </c>
       <c r="O55" s="78" t="s">
@@ -9016,7 +9114,7 @@
       <c r="J56" s="27" t="s">
         <v>548</v>
       </c>
-      <c r="K56" s="49" t="s">
+      <c r="K56" s="181" t="s">
         <v>549</v>
       </c>
       <c r="L56" s="49" t="s">
@@ -9025,7 +9123,7 @@
       <c r="M56" s="49" t="s">
         <v>550</v>
       </c>
-      <c r="N56" s="79" t="s">
+      <c r="N56" s="203" t="s">
         <v>551</v>
       </c>
       <c r="O56" s="79" t="s">
@@ -9066,7 +9164,7 @@
       <c r="J57" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K57" s="49">
+      <c r="K57" s="181">
         <v>243</v>
       </c>
       <c r="L57" s="49">
@@ -9075,7 +9173,7 @@
       <c r="M57" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N57" s="49" t="s">
+      <c r="N57" s="181" t="s">
         <v>557</v>
       </c>
       <c r="O57" s="49" t="s">
@@ -9116,7 +9214,7 @@
       <c r="J58" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K58" s="49">
+      <c r="K58" s="181">
         <v>264</v>
       </c>
       <c r="L58" s="49">
@@ -9125,7 +9223,7 @@
       <c r="M58" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N58" s="79" t="s">
+      <c r="N58" s="203" t="s">
         <v>562</v>
       </c>
       <c r="O58" s="79" t="s">
@@ -9166,7 +9264,7 @@
       <c r="J59" s="27" t="s">
         <v>567</v>
       </c>
-      <c r="K59" s="78" t="s">
+      <c r="K59" s="186" t="s">
         <v>568</v>
       </c>
       <c r="L59" s="80">
@@ -9175,7 +9273,7 @@
       <c r="M59" s="49" t="s">
         <v>569</v>
       </c>
-      <c r="N59" s="78" t="s">
+      <c r="N59" s="186" t="s">
         <v>570</v>
       </c>
       <c r="O59" s="78" t="s">
@@ -9212,7 +9310,7 @@
       <c r="J60" s="84" t="s">
         <v>69</v>
       </c>
-      <c r="K60" s="85" t="s">
+      <c r="K60" s="187" t="s">
         <v>578</v>
       </c>
       <c r="L60" s="85" t="s">
@@ -9221,7 +9319,7 @@
       <c r="M60" s="86" t="s">
         <v>579</v>
       </c>
-      <c r="N60" s="87" t="s">
+      <c r="N60" s="204" t="s">
         <v>580</v>
       </c>
       <c r="O60" s="87" t="s">
@@ -9262,7 +9360,7 @@
       <c r="J61" s="19" t="s">
         <v>587</v>
       </c>
-      <c r="K61" s="94" t="s">
+      <c r="K61" s="188" t="s">
         <v>588</v>
       </c>
       <c r="L61" s="94" t="s">
@@ -9271,7 +9369,7 @@
       <c r="M61" s="21" t="s">
         <v>590</v>
       </c>
-      <c r="N61" s="20" t="s">
+      <c r="N61" s="179" t="s">
         <v>591</v>
       </c>
       <c r="O61" s="20" t="s">
@@ -9312,7 +9410,7 @@
       <c r="J62" s="27" t="s">
         <v>601</v>
       </c>
-      <c r="K62" s="49" t="s">
+      <c r="K62" s="181" t="s">
         <v>602</v>
       </c>
       <c r="L62" s="49" t="s">
@@ -9321,7 +9419,7 @@
       <c r="M62" s="49" t="s">
         <v>603</v>
       </c>
-      <c r="N62" s="49" t="s">
+      <c r="N62" s="181" t="s">
         <v>604</v>
       </c>
       <c r="O62" s="49" t="s">
@@ -9362,7 +9460,7 @@
       <c r="J63" s="27" t="s">
         <v>613</v>
       </c>
-      <c r="K63" s="49" t="s">
+      <c r="K63" s="181" t="s">
         <v>614</v>
       </c>
       <c r="L63" s="49" t="s">
@@ -9371,7 +9469,7 @@
       <c r="M63" s="51" t="s">
         <v>615</v>
       </c>
-      <c r="N63" s="49" t="s">
+      <c r="N63" s="181" t="s">
         <v>616</v>
       </c>
       <c r="O63" s="49" t="s">
@@ -9402,14 +9500,14 @@
       <c r="H64" s="99"/>
       <c r="I64" s="102"/>
       <c r="J64" s="102"/>
-      <c r="K64" s="103" t="s">
+      <c r="K64" s="181" t="s">
         <v>621</v>
       </c>
       <c r="L64" s="103" t="s">
         <v>621</v>
       </c>
       <c r="M64" s="104"/>
-      <c r="N64" s="103" t="s">
+      <c r="N64" s="181" t="s">
         <v>622</v>
       </c>
       <c r="O64" s="103" t="s">
@@ -9434,14 +9532,14 @@
       <c r="H65" s="99"/>
       <c r="I65" s="102"/>
       <c r="J65" s="102"/>
-      <c r="K65" s="103">
+      <c r="K65" s="181">
         <v>147</v>
       </c>
       <c r="L65" s="103">
         <v>147</v>
       </c>
       <c r="M65" s="104"/>
-      <c r="N65" s="103" t="s">
+      <c r="N65" s="181" t="s">
         <v>625</v>
       </c>
       <c r="O65" s="103" t="s">
@@ -9466,14 +9564,14 @@
       <c r="H66" s="99"/>
       <c r="I66" s="102"/>
       <c r="J66" s="102"/>
-      <c r="K66" s="103" t="s">
+      <c r="K66" s="181" t="s">
         <v>628</v>
       </c>
       <c r="L66" s="103" t="s">
         <v>628</v>
       </c>
       <c r="M66" s="104"/>
-      <c r="N66" s="103" t="s">
+      <c r="N66" s="181" t="s">
         <v>629</v>
       </c>
       <c r="O66" s="103" t="s">
@@ -9508,7 +9606,7 @@
       <c r="J67" s="27" t="s">
         <v>634</v>
       </c>
-      <c r="K67" s="49">
+      <c r="K67" s="181">
         <v>150</v>
       </c>
       <c r="L67" s="49">
@@ -9517,7 +9615,7 @@
       <c r="M67" s="51" t="s">
         <v>635</v>
       </c>
-      <c r="N67" s="49" t="s">
+      <c r="N67" s="181" t="s">
         <v>636</v>
       </c>
       <c r="O67" s="49" t="s">
@@ -9558,7 +9656,7 @@
       <c r="J68" s="27" t="s">
         <v>643</v>
       </c>
-      <c r="K68" s="49">
+      <c r="K68" s="181">
         <v>151</v>
       </c>
       <c r="L68" s="49">
@@ -9567,7 +9665,7 @@
       <c r="M68" s="51" t="s">
         <v>644</v>
       </c>
-      <c r="N68" s="49" t="s">
+      <c r="N68" s="181" t="s">
         <v>645</v>
       </c>
       <c r="O68" s="49" t="s">
@@ -9608,7 +9706,7 @@
       <c r="J69" s="27" t="s">
         <v>653</v>
       </c>
-      <c r="K69" s="107" t="s">
+      <c r="K69" s="189" t="s">
         <v>654</v>
       </c>
       <c r="L69" s="107" t="s">
@@ -9617,7 +9715,7 @@
       <c r="M69" s="107" t="s">
         <v>655</v>
       </c>
-      <c r="N69" s="49" t="s">
+      <c r="N69" s="181" t="s">
         <v>656</v>
       </c>
       <c r="O69" s="49" t="s">
@@ -9658,7 +9756,7 @@
       <c r="J70" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K70" s="108" t="s">
+      <c r="K70" s="190" t="s">
         <v>663</v>
       </c>
       <c r="L70" s="108" t="s">
@@ -9667,7 +9765,7 @@
       <c r="M70" s="109" t="s">
         <v>664</v>
       </c>
-      <c r="N70" s="49" t="s">
+      <c r="N70" s="181" t="s">
         <v>665</v>
       </c>
       <c r="O70" s="49" t="s">
@@ -9708,7 +9806,7 @@
       <c r="J71" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K71" s="49">
+      <c r="K71" s="181">
         <v>157</v>
       </c>
       <c r="L71" s="49">
@@ -9717,7 +9815,7 @@
       <c r="M71" s="51" t="s">
         <v>672</v>
       </c>
-      <c r="N71" s="49" t="s">
+      <c r="N71" s="181" t="s">
         <v>673</v>
       </c>
       <c r="O71" s="49" t="s">
@@ -9758,7 +9856,7 @@
       <c r="J72" s="27" t="s">
         <v>680</v>
       </c>
-      <c r="K72" s="49">
+      <c r="K72" s="181">
         <v>162</v>
       </c>
       <c r="L72" s="49">
@@ -9767,7 +9865,7 @@
       <c r="M72" s="49" t="s">
         <v>681</v>
       </c>
-      <c r="N72" s="49" t="s">
+      <c r="N72" s="181" t="s">
         <v>682</v>
       </c>
       <c r="O72" s="49" t="s">
@@ -9808,7 +9906,7 @@
       <c r="J73" s="27" t="s">
         <v>690</v>
       </c>
-      <c r="K73" s="110" t="s">
+      <c r="K73" s="191" t="s">
         <v>691</v>
       </c>
       <c r="L73" s="110" t="s">
@@ -9817,7 +9915,7 @@
       <c r="M73" s="110" t="s">
         <v>692</v>
       </c>
-      <c r="N73" s="27" t="s">
+      <c r="N73" s="185" t="s">
         <v>693</v>
       </c>
       <c r="O73" s="27" t="s">
@@ -9848,7 +9946,7 @@
       <c r="H74" s="99"/>
       <c r="I74" s="102"/>
       <c r="J74" s="102"/>
-      <c r="K74" s="111">
+      <c r="K74" s="191">
         <v>172</v>
       </c>
       <c r="L74" s="111">
@@ -9857,7 +9955,7 @@
       <c r="M74" s="111" t="s">
         <v>697</v>
       </c>
-      <c r="N74" s="102" t="s">
+      <c r="N74" s="185" t="s">
         <v>698</v>
       </c>
       <c r="O74" s="102" t="s">
@@ -9884,7 +9982,7 @@
       <c r="H75" s="99"/>
       <c r="I75" s="102"/>
       <c r="J75" s="102"/>
-      <c r="K75" s="111">
+      <c r="K75" s="191">
         <v>173</v>
       </c>
       <c r="L75" s="111">
@@ -9893,7 +9991,7 @@
       <c r="M75" s="111" t="s">
         <v>702</v>
       </c>
-      <c r="N75" s="102" t="s">
+      <c r="N75" s="185" t="s">
         <v>703</v>
       </c>
       <c r="O75" s="102" t="s">
@@ -9928,7 +10026,7 @@
       <c r="J76" s="27" t="s">
         <v>708</v>
       </c>
-      <c r="K76" s="49" t="s">
+      <c r="K76" s="181" t="s">
         <v>709</v>
       </c>
       <c r="L76" s="49" t="s">
@@ -9937,7 +10035,7 @@
       <c r="M76" s="49" t="s">
         <v>710</v>
       </c>
-      <c r="N76" s="49" t="s">
+      <c r="N76" s="181" t="s">
         <v>711</v>
       </c>
       <c r="O76" s="49" t="s">
@@ -9978,7 +10076,7 @@
       <c r="J77" s="27" t="s">
         <v>689</v>
       </c>
-      <c r="K77" s="49">
+      <c r="K77" s="181">
         <v>180</v>
       </c>
       <c r="L77" s="49">
@@ -9987,7 +10085,7 @@
       <c r="M77" s="49" t="s">
         <v>719</v>
       </c>
-      <c r="N77" s="49" t="s">
+      <c r="N77" s="181" t="s">
         <v>720</v>
       </c>
       <c r="O77" s="49" t="s">
@@ -10028,7 +10126,7 @@
       <c r="J78" s="27" t="s">
         <v>727</v>
       </c>
-      <c r="K78" s="107" t="s">
+      <c r="K78" s="189" t="s">
         <v>728</v>
       </c>
       <c r="L78" s="107" t="s">
@@ -10037,7 +10135,7 @@
       <c r="M78" s="49" t="s">
         <v>729</v>
       </c>
-      <c r="N78" s="49" t="s">
+      <c r="N78" s="181" t="s">
         <v>730</v>
       </c>
       <c r="O78" s="49" t="s">
@@ -10078,7 +10176,7 @@
       <c r="J79" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K79" s="49">
+      <c r="K79" s="181">
         <v>183</v>
       </c>
       <c r="L79" s="49">
@@ -10087,7 +10185,7 @@
       <c r="M79" s="49" t="s">
         <v>736</v>
       </c>
-      <c r="N79" s="49" t="s">
+      <c r="N79" s="181" t="s">
         <v>737</v>
       </c>
       <c r="O79" s="49" t="s">
@@ -10128,7 +10226,7 @@
       <c r="J80" s="27" t="s">
         <v>743</v>
       </c>
-      <c r="K80" s="49">
+      <c r="K80" s="181">
         <v>185</v>
       </c>
       <c r="L80" s="49">
@@ -10137,7 +10235,7 @@
       <c r="M80" s="49" t="s">
         <v>744</v>
       </c>
-      <c r="N80" s="49" t="s">
+      <c r="N80" s="181" t="s">
         <v>745</v>
       </c>
       <c r="O80" s="49" t="s">
@@ -10170,7 +10268,7 @@
       <c r="H81" s="99"/>
       <c r="I81" s="102"/>
       <c r="J81" s="102"/>
-      <c r="K81" s="103">
+      <c r="K81" s="181">
         <v>186</v>
       </c>
       <c r="L81" s="103">
@@ -10179,7 +10277,7 @@
       <c r="M81" s="103" t="s">
         <v>749</v>
       </c>
-      <c r="N81" s="103" t="s">
+      <c r="N81" s="181" t="s">
         <v>750</v>
       </c>
       <c r="O81" s="103" t="s">
@@ -10206,14 +10304,14 @@
       <c r="H82" s="99"/>
       <c r="I82" s="102"/>
       <c r="J82" s="102"/>
-      <c r="K82" s="103">
+      <c r="K82" s="181">
         <v>189</v>
       </c>
       <c r="L82" s="103">
         <v>189</v>
       </c>
       <c r="M82" s="103"/>
-      <c r="N82" s="103" t="s">
+      <c r="N82" s="181" t="s">
         <v>754</v>
       </c>
       <c r="O82" s="103" t="s">
@@ -10248,7 +10346,7 @@
       <c r="J83" s="27">
         <v>188</v>
       </c>
-      <c r="K83" s="49">
+      <c r="K83" s="181">
         <v>188</v>
       </c>
       <c r="L83" s="49">
@@ -10257,7 +10355,7 @@
       <c r="M83" s="49" t="s">
         <v>761</v>
       </c>
-      <c r="N83" s="49" t="s">
+      <c r="N83" s="181" t="s">
         <v>762</v>
       </c>
       <c r="O83" s="49" t="s">
@@ -10290,7 +10388,7 @@
       <c r="H84" s="99"/>
       <c r="I84" s="102"/>
       <c r="J84" s="102"/>
-      <c r="K84" s="103" t="s">
+      <c r="K84" s="181" t="s">
         <v>768</v>
       </c>
       <c r="L84" s="103" t="s">
@@ -10299,7 +10397,7 @@
       <c r="M84" s="103" t="s">
         <v>769</v>
       </c>
-      <c r="N84" s="103" t="s">
+      <c r="N84" s="181" t="s">
         <v>770</v>
       </c>
       <c r="O84" s="103" t="s">
@@ -10328,14 +10426,14 @@
       <c r="H85" s="99"/>
       <c r="I85" s="102"/>
       <c r="J85" s="102"/>
-      <c r="K85" s="103">
+      <c r="K85" s="181">
         <v>156</v>
       </c>
       <c r="L85" s="103">
         <v>156</v>
       </c>
       <c r="M85" s="103"/>
-      <c r="N85" s="103" t="s">
+      <c r="N85" s="181" t="s">
         <v>775</v>
       </c>
       <c r="O85" s="103" t="s">
@@ -10362,7 +10460,7 @@
       <c r="H86" s="99"/>
       <c r="I86" s="102"/>
       <c r="J86" s="102"/>
-      <c r="K86" s="103">
+      <c r="K86" s="181">
         <v>161</v>
       </c>
       <c r="L86" s="103">
@@ -10371,7 +10469,7 @@
       <c r="M86" s="103" t="s">
         <v>779</v>
       </c>
-      <c r="N86" s="103" t="s">
+      <c r="N86" s="181" t="s">
         <v>780</v>
       </c>
       <c r="O86" s="103" t="s">
@@ -10402,14 +10500,14 @@
       <c r="H87" s="99"/>
       <c r="I87" s="102"/>
       <c r="J87" s="102"/>
-      <c r="K87" s="103">
+      <c r="K87" s="181">
         <v>193</v>
       </c>
       <c r="L87" s="103">
         <v>193</v>
       </c>
       <c r="M87" s="103"/>
-      <c r="N87" s="103" t="s">
+      <c r="N87" s="181" t="s">
         <v>785</v>
       </c>
       <c r="O87" s="103" t="s">
@@ -10436,10 +10534,10 @@
       <c r="H88" s="99"/>
       <c r="I88" s="102"/>
       <c r="J88" s="102"/>
-      <c r="K88" s="103"/>
+      <c r="K88" s="181"/>
       <c r="L88" s="103"/>
       <c r="M88" s="103"/>
-      <c r="N88" s="103" t="s">
+      <c r="N88" s="181" t="s">
         <v>789</v>
       </c>
       <c r="O88" s="103" t="s">
@@ -10474,7 +10572,7 @@
       <c r="J89" s="27" t="s">
         <v>796</v>
       </c>
-      <c r="K89" s="49" t="s">
+      <c r="K89" s="181" t="s">
         <v>797</v>
       </c>
       <c r="L89" s="49" t="s">
@@ -10483,7 +10581,7 @@
       <c r="M89" s="49" t="s">
         <v>798</v>
       </c>
-      <c r="N89" s="49" t="s">
+      <c r="N89" s="181" t="s">
         <v>799</v>
       </c>
       <c r="O89" s="49" t="s">
@@ -10514,7 +10612,7 @@
       <c r="H90" s="99"/>
       <c r="I90" s="102"/>
       <c r="J90" s="102"/>
-      <c r="K90" s="103">
+      <c r="K90" s="181">
         <v>201</v>
       </c>
       <c r="L90" s="103">
@@ -10523,7 +10621,7 @@
       <c r="M90" s="103" t="s">
         <v>804</v>
       </c>
-      <c r="N90" s="103" t="s">
+      <c r="N90" s="181" t="s">
         <v>805</v>
       </c>
       <c r="O90" s="103" t="s">
@@ -10548,14 +10646,14 @@
       <c r="H91" s="99"/>
       <c r="I91" s="102"/>
       <c r="J91" s="114"/>
-      <c r="K91" s="103" t="s">
+      <c r="K91" s="181" t="s">
         <v>808</v>
       </c>
       <c r="L91" s="103" t="s">
         <v>808</v>
       </c>
       <c r="M91" s="103"/>
-      <c r="N91" s="103" t="s">
+      <c r="N91" s="181" t="s">
         <v>809</v>
       </c>
       <c r="O91" s="103" t="s">
@@ -10582,14 +10680,14 @@
       <c r="H92" s="99"/>
       <c r="I92" s="102"/>
       <c r="J92" s="102"/>
-      <c r="K92" s="103">
+      <c r="K92" s="181">
         <v>203</v>
       </c>
       <c r="L92" s="103">
         <v>203</v>
       </c>
       <c r="M92" s="103"/>
-      <c r="N92" s="103" t="s">
+      <c r="N92" s="181" t="s">
         <v>813</v>
       </c>
       <c r="O92" s="103" t="s">
@@ -10624,7 +10722,7 @@
       <c r="J93" s="27" t="s">
         <v>795</v>
       </c>
-      <c r="K93" s="49" t="s">
+      <c r="K93" s="181" t="s">
         <v>820</v>
       </c>
       <c r="L93" s="49" t="s">
@@ -10633,7 +10731,7 @@
       <c r="M93" s="49" t="s">
         <v>821</v>
       </c>
-      <c r="N93" s="49" t="s">
+      <c r="N93" s="181" t="s">
         <v>822</v>
       </c>
       <c r="O93" s="49" t="s">
@@ -10672,7 +10770,7 @@
       <c r="J94" s="53" t="s">
         <v>830</v>
       </c>
-      <c r="K94" s="54" t="s">
+      <c r="K94" s="184" t="s">
         <v>831</v>
       </c>
       <c r="L94" s="54" t="s">
@@ -10681,7 +10779,7 @@
       <c r="M94" s="54" t="s">
         <v>832</v>
       </c>
-      <c r="N94" s="54" t="s">
+      <c r="N94" s="184" t="s">
         <v>833</v>
       </c>
       <c r="O94" s="54" t="s">
@@ -10722,7 +10820,7 @@
       <c r="J95" s="27" t="s">
         <v>841</v>
       </c>
-      <c r="K95" s="49" t="s">
+      <c r="K95" s="181" t="s">
         <v>842</v>
       </c>
       <c r="L95" s="49" t="s">
@@ -10731,7 +10829,7 @@
       <c r="M95" s="107" t="s">
         <v>843</v>
       </c>
-      <c r="N95" s="49" t="s">
+      <c r="N95" s="181" t="s">
         <v>844</v>
       </c>
       <c r="O95" s="49" t="s">
@@ -10772,7 +10870,7 @@
       <c r="J96" s="27" t="s">
         <v>547</v>
       </c>
-      <c r="K96" s="49">
+      <c r="K96" s="181">
         <v>250</v>
       </c>
       <c r="L96" s="49">
@@ -10781,7 +10879,7 @@
       <c r="M96" s="49" t="s">
         <v>853</v>
       </c>
-      <c r="N96" s="79" t="s">
+      <c r="N96" s="203" t="s">
         <v>854</v>
       </c>
       <c r="O96" s="79" t="s">
@@ -10797,103 +10895,103 @@
         <v>856</v>
       </c>
     </row>
-    <row r="97" spans="1:18" s="163" customFormat="1" ht="104" x14ac:dyDescent="0.2">
-      <c r="A97" s="153" t="s">
+    <row r="97" spans="1:18" s="160" customFormat="1" ht="104" x14ac:dyDescent="0.2">
+      <c r="A97" s="150" t="s">
         <v>857</v>
       </c>
-      <c r="B97" s="154" t="s">
+      <c r="B97" s="151" t="s">
         <v>858</v>
       </c>
-      <c r="C97" s="155" t="s">
+      <c r="C97" s="152" t="s">
         <v>859</v>
       </c>
-      <c r="D97" s="156"/>
-      <c r="E97" s="157" t="s">
+      <c r="D97" s="153"/>
+      <c r="E97" s="154" t="s">
         <v>490</v>
       </c>
-      <c r="F97" s="158" t="s">
+      <c r="F97" s="155" t="s">
         <v>860</v>
       </c>
-      <c r="G97" s="159"/>
-      <c r="H97" s="159"/>
-      <c r="I97" s="160" t="s">
+      <c r="G97" s="156"/>
+      <c r="H97" s="156"/>
+      <c r="I97" s="157" t="s">
         <v>861</v>
       </c>
-      <c r="J97" s="160" t="s">
+      <c r="J97" s="157" t="s">
         <v>862</v>
       </c>
-      <c r="K97" s="164" t="s">
+      <c r="K97" s="186" t="s">
         <v>863</v>
       </c>
-      <c r="L97" s="164" t="s">
+      <c r="L97" s="161" t="s">
         <v>864</v>
       </c>
-      <c r="M97" s="161" t="s">
+      <c r="M97" s="158" t="s">
         <v>865</v>
       </c>
-      <c r="N97" s="165" t="s">
+      <c r="N97" s="205" t="s">
         <v>866</v>
       </c>
-      <c r="O97" s="165" t="s">
+      <c r="O97" s="162" t="s">
         <v>867</v>
       </c>
-      <c r="P97" s="162" t="s">
+      <c r="P97" s="159" t="s">
         <v>868</v>
       </c>
-      <c r="Q97" s="162" t="s">
+      <c r="Q97" s="159" t="s">
         <v>869</v>
       </c>
-      <c r="R97" s="166" t="s">
+      <c r="R97" s="163" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="98" spans="1:18" s="163" customFormat="1" ht="52" x14ac:dyDescent="0.2">
-      <c r="A98" s="153" t="s">
+    <row r="98" spans="1:18" s="160" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+      <c r="A98" s="150" t="s">
         <v>871</v>
       </c>
-      <c r="B98" s="154" t="s">
+      <c r="B98" s="151" t="s">
         <v>872</v>
       </c>
-      <c r="C98" s="155" t="s">
+      <c r="C98" s="152" t="s">
         <v>873</v>
       </c>
-      <c r="D98" s="156"/>
-      <c r="E98" s="157" t="s">
+      <c r="D98" s="153"/>
+      <c r="E98" s="154" t="s">
         <v>533</v>
       </c>
-      <c r="F98" s="158" t="s">
+      <c r="F98" s="155" t="s">
         <v>874</v>
       </c>
-      <c r="G98" s="159"/>
-      <c r="H98" s="159"/>
-      <c r="I98" s="160" t="s">
+      <c r="G98" s="156"/>
+      <c r="H98" s="156"/>
+      <c r="I98" s="157" t="s">
         <v>875</v>
       </c>
-      <c r="J98" s="160" t="s">
+      <c r="J98" s="157" t="s">
         <v>876</v>
       </c>
-      <c r="K98" s="161" t="s">
+      <c r="K98" s="181" t="s">
         <v>877</v>
       </c>
-      <c r="L98" s="161" t="s">
+      <c r="L98" s="158" t="s">
         <v>877</v>
       </c>
-      <c r="M98" s="161" t="s">
+      <c r="M98" s="158" t="s">
         <v>878</v>
       </c>
-      <c r="N98" s="161" t="s">
+      <c r="N98" s="181" t="s">
         <v>879</v>
       </c>
-      <c r="O98" s="161" t="s">
+      <c r="O98" s="158" t="s">
         <v>879</v>
       </c>
-      <c r="P98" s="162" t="s">
+      <c r="P98" s="159" t="s">
         <v>880</v>
       </c>
-      <c r="Q98" s="162" t="s">
+      <c r="Q98" s="159" t="s">
         <v>881</v>
       </c>
-      <c r="R98" s="166" t="s">
+      <c r="R98" s="163" t="s">
         <v>882</v>
       </c>
     </row>
@@ -10922,7 +11020,7 @@
       <c r="J99" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K99" s="27" t="s">
+      <c r="K99" s="185" t="s">
         <v>887</v>
       </c>
       <c r="L99" s="27">
@@ -10931,7 +11029,7 @@
       <c r="M99" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N99" s="49" t="s">
+      <c r="N99" s="181" t="s">
         <v>888</v>
       </c>
       <c r="O99" s="49" t="s">
@@ -10972,7 +11070,7 @@
       <c r="J100" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K100" s="49" t="s">
+      <c r="K100" s="181" t="s">
         <v>893</v>
       </c>
       <c r="L100" s="49">
@@ -10981,7 +11079,7 @@
       <c r="M100" s="49" t="s">
         <v>894</v>
       </c>
-      <c r="N100" s="49" t="s">
+      <c r="N100" s="181" t="s">
         <v>895</v>
       </c>
       <c r="O100" s="49" t="s">
@@ -11022,7 +11120,7 @@
       <c r="J101" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K101" s="49">
+      <c r="K101" s="181">
         <v>295</v>
       </c>
       <c r="L101" s="49">
@@ -11031,7 +11129,7 @@
       <c r="M101" s="49" t="s">
         <v>900</v>
       </c>
-      <c r="N101" s="49" t="s">
+      <c r="N101" s="181" t="s">
         <v>901</v>
       </c>
       <c r="O101" s="49" t="s">
@@ -11072,7 +11170,7 @@
       <c r="J102" s="27" t="s">
         <v>907</v>
       </c>
-      <c r="K102" s="49">
+      <c r="K102" s="181">
         <v>345</v>
       </c>
       <c r="L102" s="49">
@@ -11081,7 +11179,7 @@
       <c r="M102" s="49" t="s">
         <v>908</v>
       </c>
-      <c r="N102" s="49" t="s">
+      <c r="N102" s="181" t="s">
         <v>909</v>
       </c>
       <c r="O102" s="49" t="s">
@@ -11112,17 +11210,17 @@
       <c r="F103" s="120" t="s">
         <v>130</v>
       </c>
-      <c r="G103" s="121" t="s">
+      <c r="G103" s="176" t="s">
         <v>913</v>
       </c>
-      <c r="H103" s="119"/>
+      <c r="H103" s="35"/>
       <c r="I103" s="27" t="s">
         <v>69</v>
       </c>
       <c r="J103" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K103" s="51" t="s">
+      <c r="K103" s="183" t="s">
         <v>914</v>
       </c>
       <c r="L103" s="51" t="s">
@@ -11131,7 +11229,7 @@
       <c r="M103" s="49" t="s">
         <v>916</v>
       </c>
-      <c r="N103" s="49" t="s">
+      <c r="N103" s="181" t="s">
         <v>917</v>
       </c>
       <c r="O103" s="49" t="s">
@@ -11172,7 +11270,7 @@
       <c r="J104" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K104" s="107" t="s">
+      <c r="K104" s="189" t="s">
         <v>922</v>
       </c>
       <c r="L104" s="107" t="s">
@@ -11181,7 +11279,7 @@
       <c r="M104" s="49" t="s">
         <v>923</v>
       </c>
-      <c r="N104" s="49" t="s">
+      <c r="N104" s="181" t="s">
         <v>924</v>
       </c>
       <c r="O104" s="49" t="s">
@@ -11222,7 +11320,7 @@
       <c r="J105" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K105" s="49">
+      <c r="K105" s="181">
         <v>332</v>
       </c>
       <c r="L105" s="49">
@@ -11231,7 +11329,7 @@
       <c r="M105" s="49" t="s">
         <v>929</v>
       </c>
-      <c r="N105" s="49" t="s">
+      <c r="N105" s="181" t="s">
         <v>930</v>
       </c>
       <c r="O105" s="49" t="s">
@@ -11272,7 +11370,7 @@
       <c r="J106" s="27" t="s">
         <v>906</v>
       </c>
-      <c r="K106" s="49">
+      <c r="K106" s="181">
         <v>340</v>
       </c>
       <c r="L106" s="49">
@@ -11281,7 +11379,7 @@
       <c r="M106" s="49" t="s">
         <v>936</v>
       </c>
-      <c r="N106" s="49" t="s">
+      <c r="N106" s="181" t="s">
         <v>937</v>
       </c>
       <c r="O106" s="49" t="s">
@@ -11312,17 +11410,17 @@
       <c r="F107" s="120" t="s">
         <v>243</v>
       </c>
-      <c r="G107" s="121" t="s">
+      <c r="G107" s="176" t="s">
         <v>941</v>
       </c>
-      <c r="H107" s="119"/>
+      <c r="H107" s="35"/>
       <c r="I107" s="27" t="s">
         <v>69</v>
       </c>
       <c r="J107" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K107" s="51" t="s">
+      <c r="K107" s="183" t="s">
         <v>942</v>
       </c>
       <c r="L107" s="51" t="s">
@@ -11331,7 +11429,7 @@
       <c r="M107" s="49" t="s">
         <v>944</v>
       </c>
-      <c r="N107" s="49" t="s">
+      <c r="N107" s="181" t="s">
         <v>945</v>
       </c>
       <c r="O107" s="49" t="s">
@@ -11372,7 +11470,7 @@
       <c r="J108" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K108" s="27" t="s">
+      <c r="K108" s="185" t="s">
         <v>950</v>
       </c>
       <c r="L108" s="27" t="s">
@@ -11381,10 +11479,10 @@
       <c r="M108" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N108" s="122" t="s">
+      <c r="N108" s="200" t="s">
         <v>951</v>
       </c>
-      <c r="O108" s="122" t="s">
+      <c r="O108" s="121" t="s">
         <v>952</v>
       </c>
       <c r="P108" s="50" t="s">
@@ -11422,7 +11520,7 @@
       <c r="J109" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K109" s="107" t="s">
+      <c r="K109" s="189" t="s">
         <v>957</v>
       </c>
       <c r="L109" s="50" t="s">
@@ -11431,7 +11529,7 @@
       <c r="M109" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N109" s="49" t="s">
+      <c r="N109" s="181" t="s">
         <v>958</v>
       </c>
       <c r="O109" s="49" t="s">
@@ -11472,7 +11570,7 @@
       <c r="J110" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K110" s="123" t="s">
+      <c r="K110" s="192" t="s">
         <v>963</v>
       </c>
       <c r="L110" s="50" t="s">
@@ -11481,7 +11579,7 @@
       <c r="M110" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N110" s="49" t="s">
+      <c r="N110" s="181" t="s">
         <v>964</v>
       </c>
       <c r="O110" s="50" t="s">
@@ -11507,7 +11605,7 @@
       <c r="C111" s="52"/>
       <c r="D111" s="60"/>
       <c r="E111" s="61"/>
-      <c r="F111" s="124" t="s">
+      <c r="F111" s="122" t="s">
         <v>325</v>
       </c>
       <c r="G111" s="95" t="s">
@@ -11520,7 +11618,7 @@
       <c r="J111" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K111" s="125">
+      <c r="K111" s="193">
         <v>307.39999999999998</v>
       </c>
       <c r="L111" s="50" t="s">
@@ -11529,7 +11627,7 @@
       <c r="M111" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N111" s="54" t="s">
+      <c r="N111" s="184" t="s">
         <v>968</v>
       </c>
       <c r="O111" s="54" t="s">
@@ -11555,7 +11653,7 @@
       <c r="C112" s="52"/>
       <c r="D112" s="60"/>
       <c r="E112" s="61"/>
-      <c r="F112" s="124" t="s">
+      <c r="F112" s="122" t="s">
         <v>333</v>
       </c>
       <c r="G112" s="95" t="s">
@@ -11568,16 +11666,16 @@
       <c r="J112" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K112" s="126">
+      <c r="K112" s="194">
         <v>346</v>
       </c>
-      <c r="L112" s="126">
+      <c r="L112" s="123">
         <v>346</v>
       </c>
       <c r="M112" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N112" s="54" t="s">
+      <c r="N112" s="184" t="s">
         <v>972</v>
       </c>
       <c r="O112" s="54" t="s">
@@ -11603,7 +11701,7 @@
       <c r="C113" s="52"/>
       <c r="D113" s="60"/>
       <c r="E113" s="61"/>
-      <c r="F113" s="124" t="s">
+      <c r="F113" s="122" t="s">
         <v>752</v>
       </c>
       <c r="G113" s="1" t="s">
@@ -11616,16 +11714,16 @@
       <c r="J113" s="53" t="s">
         <v>976</v>
       </c>
-      <c r="K113" s="127" t="s">
+      <c r="K113" s="195" t="s">
         <v>977</v>
       </c>
-      <c r="L113" s="127" t="s">
+      <c r="L113" s="124" t="s">
         <v>977</v>
       </c>
       <c r="M113" s="53" t="s">
         <v>978</v>
       </c>
-      <c r="N113" s="54" t="s">
+      <c r="N113" s="184" t="s">
         <v>979</v>
       </c>
       <c r="O113" s="54" t="s">
@@ -11662,16 +11760,16 @@
       <c r="J114" s="53" t="s">
         <v>984</v>
       </c>
-      <c r="K114" s="128" t="s">
+      <c r="K114" s="196" t="s">
         <v>985</v>
       </c>
-      <c r="L114" s="128" t="s">
+      <c r="L114" s="125" t="s">
         <v>986</v>
       </c>
       <c r="M114" s="53" t="s">
         <v>987</v>
       </c>
-      <c r="N114" s="54" t="s">
+      <c r="N114" s="184" t="s">
         <v>988</v>
       </c>
       <c r="O114" s="54" t="s">
@@ -11712,7 +11810,7 @@
       <c r="J115" s="27" t="s">
         <v>998</v>
       </c>
-      <c r="K115" s="49" t="s">
+      <c r="K115" s="181" t="s">
         <v>999</v>
       </c>
       <c r="L115" s="49" t="s">
@@ -11721,7 +11819,7 @@
       <c r="M115" s="49" t="s">
         <v>1000</v>
       </c>
-      <c r="N115" s="49" t="s">
+      <c r="N115" s="181" t="s">
         <v>1001</v>
       </c>
       <c r="O115" s="49" t="s">
@@ -11762,7 +11860,7 @@
       <c r="J116" s="27" t="s">
         <v>417</v>
       </c>
-      <c r="K116" s="49">
+      <c r="K116" s="181">
         <v>365</v>
       </c>
       <c r="L116" s="49">
@@ -11771,7 +11869,7 @@
       <c r="M116" s="49" t="s">
         <v>1008</v>
       </c>
-      <c r="N116" s="49" t="s">
+      <c r="N116" s="181" t="s">
         <v>1009</v>
       </c>
       <c r="O116" s="49" t="s">
@@ -11812,7 +11910,7 @@
       <c r="J117" s="27" t="s">
         <v>1007</v>
       </c>
-      <c r="K117" s="49">
+      <c r="K117" s="181">
         <v>366</v>
       </c>
       <c r="L117" s="49">
@@ -11821,7 +11919,7 @@
       <c r="M117" s="49" t="s">
         <v>1015</v>
       </c>
-      <c r="N117" s="49" t="s">
+      <c r="N117" s="181" t="s">
         <v>1016</v>
       </c>
       <c r="O117" s="49" t="s">
@@ -11847,7 +11945,7 @@
       <c r="C118" s="52"/>
       <c r="D118" s="60"/>
       <c r="E118" s="61"/>
-      <c r="F118" s="124" t="s">
+      <c r="F118" s="122" t="s">
         <v>107</v>
       </c>
       <c r="G118" s="95" t="s">
@@ -11860,7 +11958,7 @@
       <c r="J118" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K118" s="54">
+      <c r="K118" s="184">
         <v>367.4</v>
       </c>
       <c r="L118" s="50" t="s">
@@ -11869,7 +11967,7 @@
       <c r="M118" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N118" s="54" t="s">
+      <c r="N118" s="184" t="s">
         <v>1020</v>
       </c>
       <c r="O118" s="50" t="s">
@@ -11895,7 +11993,7 @@
       <c r="C119" s="52"/>
       <c r="D119" s="60"/>
       <c r="E119" s="61"/>
-      <c r="F119" s="124" t="s">
+      <c r="F119" s="122" t="s">
         <v>117</v>
       </c>
       <c r="G119" s="95" t="s">
@@ -11908,7 +12006,7 @@
       <c r="J119" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K119" s="54">
+      <c r="K119" s="184">
         <v>389</v>
       </c>
       <c r="L119" s="54">
@@ -11917,7 +12015,7 @@
       <c r="M119" s="53" t="s">
         <v>1024</v>
       </c>
-      <c r="N119" s="54" t="s">
+      <c r="N119" s="184" t="s">
         <v>1025</v>
       </c>
       <c r="O119" s="54" t="s">
@@ -11943,7 +12041,7 @@
       <c r="C120" s="52"/>
       <c r="D120" s="60"/>
       <c r="E120" s="61"/>
-      <c r="F120" s="124"/>
+      <c r="F120" s="122"/>
       <c r="G120" s="95" t="s">
         <v>1028</v>
       </c>
@@ -11954,7 +12052,7 @@
       <c r="J120" s="53" t="s">
         <v>1014</v>
       </c>
-      <c r="K120" s="54" t="s">
+      <c r="K120" s="184" t="s">
         <v>1029</v>
       </c>
       <c r="L120" s="54" t="s">
@@ -11963,7 +12061,7 @@
       <c r="M120" s="54" t="s">
         <v>1031</v>
       </c>
-      <c r="N120" s="54" t="s">
+      <c r="N120" s="184" t="s">
         <v>1032</v>
       </c>
       <c r="O120" s="54" t="s">
@@ -11979,53 +12077,53 @@
         <v>69</v>
       </c>
     </row>
-    <row r="121" spans="1:18" s="163" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="A121" s="153" t="s">
+    <row r="121" spans="1:18" s="160" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A121" s="150" t="s">
         <v>1034</v>
       </c>
-      <c r="B121" s="154" t="s">
+      <c r="B121" s="151" t="s">
         <v>1035</v>
       </c>
-      <c r="C121" s="155" t="s">
+      <c r="C121" s="152" t="s">
         <v>1036</v>
       </c>
-      <c r="D121" s="156"/>
-      <c r="E121" s="157" t="s">
+      <c r="D121" s="153"/>
+      <c r="E121" s="154" t="s">
         <v>1037</v>
       </c>
-      <c r="F121" s="158" t="s">
+      <c r="F121" s="155" t="s">
         <v>1038</v>
       </c>
-      <c r="G121" s="159"/>
-      <c r="H121" s="159"/>
-      <c r="I121" s="160" t="s">
+      <c r="G121" s="156"/>
+      <c r="H121" s="156"/>
+      <c r="I121" s="157" t="s">
         <v>1039</v>
       </c>
-      <c r="J121" s="160" t="s">
+      <c r="J121" s="157" t="s">
         <v>1040</v>
       </c>
-      <c r="K121" s="161" t="s">
+      <c r="K121" s="181" t="s">
         <v>1041</v>
       </c>
-      <c r="L121" s="161" t="s">
+      <c r="L121" s="158" t="s">
         <v>1041</v>
       </c>
-      <c r="M121" s="161" t="s">
+      <c r="M121" s="158" t="s">
         <v>1042</v>
       </c>
-      <c r="N121" s="161" t="s">
+      <c r="N121" s="181" t="s">
         <v>1043</v>
       </c>
-      <c r="O121" s="161" t="s">
+      <c r="O121" s="158" t="s">
         <v>1043</v>
       </c>
-      <c r="P121" s="162" t="s">
+      <c r="P121" s="159" t="s">
         <v>1042</v>
       </c>
-      <c r="Q121" s="162" t="s">
+      <c r="Q121" s="159" t="s">
         <v>1044</v>
       </c>
-      <c r="R121" s="166" t="s">
+      <c r="R121" s="163" t="s">
         <v>1045</v>
       </c>
     </row>
@@ -12054,7 +12152,7 @@
       <c r="J122" s="27" t="s">
         <v>1051</v>
       </c>
-      <c r="K122" s="49" t="s">
+      <c r="K122" s="181" t="s">
         <v>1052</v>
       </c>
       <c r="L122" s="49" t="s">
@@ -12063,7 +12161,7 @@
       <c r="M122" s="49" t="s">
         <v>1053</v>
       </c>
-      <c r="N122" s="49" t="s">
+      <c r="N122" s="181" t="s">
         <v>1054</v>
       </c>
       <c r="O122" s="49" t="s">
@@ -12089,7 +12187,7 @@
       <c r="C123" s="52"/>
       <c r="D123" s="60"/>
       <c r="E123" s="61"/>
-      <c r="F123" s="124" t="s">
+      <c r="F123" s="122" t="s">
         <v>62</v>
       </c>
       <c r="G123" s="95" t="s">
@@ -12102,7 +12200,7 @@
       <c r="J123" s="53" t="s">
         <v>1061</v>
       </c>
-      <c r="K123" s="54" t="s">
+      <c r="K123" s="184" t="s">
         <v>1062</v>
       </c>
       <c r="L123" s="54" t="s">
@@ -12111,7 +12209,7 @@
       <c r="M123" s="54" t="s">
         <v>1063</v>
       </c>
-      <c r="N123" s="54" t="s">
+      <c r="N123" s="184" t="s">
         <v>1064</v>
       </c>
       <c r="O123" s="54" t="s">
@@ -12152,7 +12250,7 @@
       <c r="J124" s="27" t="s">
         <v>1072</v>
       </c>
-      <c r="K124" s="51" t="s">
+      <c r="K124" s="183" t="s">
         <v>1073</v>
       </c>
       <c r="L124" s="51" t="s">
@@ -12161,7 +12259,7 @@
       <c r="M124" s="49" t="s">
         <v>1074</v>
       </c>
-      <c r="N124" s="49" t="s">
+      <c r="N124" s="181" t="s">
         <v>1075</v>
       </c>
       <c r="O124" s="49" t="s">
@@ -12202,7 +12300,7 @@
       <c r="J125" s="27" t="s">
         <v>1084</v>
       </c>
-      <c r="K125" s="49" t="s">
+      <c r="K125" s="181" t="s">
         <v>1085</v>
       </c>
       <c r="L125" s="49" t="s">
@@ -12211,7 +12309,7 @@
       <c r="M125" s="49" t="s">
         <v>1086</v>
       </c>
-      <c r="N125" s="49" t="s">
+      <c r="N125" s="181" t="s">
         <v>1087</v>
       </c>
       <c r="O125" s="49" t="s">
@@ -12252,16 +12350,16 @@
       <c r="J126" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K126" s="129" t="s">
+      <c r="K126" s="197" t="s">
         <v>1094</v>
       </c>
-      <c r="L126" s="129" t="s">
+      <c r="L126" s="126" t="s">
         <v>1094</v>
       </c>
       <c r="M126" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N126" s="49" t="s">
+      <c r="N126" s="181" t="s">
         <v>1095</v>
       </c>
       <c r="O126" s="49" t="s">
@@ -12278,36 +12376,36 @@
       </c>
     </row>
     <row r="127" spans="1:18" ht="65" x14ac:dyDescent="0.2">
-      <c r="A127" s="130" t="s">
+      <c r="A127" s="127" t="s">
         <v>1096</v>
       </c>
       <c r="B127" s="9" t="s">
         <v>1097</v>
       </c>
-      <c r="C127" s="131"/>
-      <c r="D127" s="130"/>
+      <c r="C127" s="128"/>
+      <c r="D127" s="127"/>
       <c r="E127" s="76"/>
       <c r="F127" s="76"/>
       <c r="G127" s="81" t="s">
         <v>1098</v>
       </c>
       <c r="H127" s="76"/>
-      <c r="I127" s="132" t="s">
+      <c r="I127" s="129" t="s">
         <v>1099</v>
       </c>
       <c r="J127" s="53" t="s">
         <v>1100</v>
       </c>
-      <c r="K127" s="133" t="s">
+      <c r="K127" s="198" t="s">
         <v>1101</v>
       </c>
-      <c r="L127" s="133" t="s">
+      <c r="L127" s="130" t="s">
         <v>1101</v>
       </c>
       <c r="M127" s="53" t="s">
         <v>1102</v>
       </c>
-      <c r="N127" s="54" t="s">
+      <c r="N127" s="184" t="s">
         <v>1103</v>
       </c>
       <c r="O127" s="54" t="s">
@@ -12323,53 +12421,53 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="128" spans="1:18" s="163" customFormat="1" ht="52" x14ac:dyDescent="0.2">
-      <c r="A128" s="153" t="s">
+    <row r="128" spans="1:18" s="160" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+      <c r="A128" s="150" t="s">
         <v>1106</v>
       </c>
-      <c r="B128" s="154" t="s">
+      <c r="B128" s="151" t="s">
         <v>1107</v>
       </c>
-      <c r="C128" s="155" t="s">
+      <c r="C128" s="152" t="s">
         <v>1108</v>
       </c>
-      <c r="D128" s="156"/>
-      <c r="E128" s="157" t="s">
+      <c r="D128" s="153"/>
+      <c r="E128" s="154" t="s">
         <v>1109</v>
       </c>
-      <c r="F128" s="158" t="s">
+      <c r="F128" s="155" t="s">
         <v>1110</v>
       </c>
-      <c r="G128" s="159"/>
-      <c r="H128" s="159"/>
-      <c r="I128" s="160" t="s">
+      <c r="G128" s="156"/>
+      <c r="H128" s="156"/>
+      <c r="I128" s="157" t="s">
         <v>1111</v>
       </c>
-      <c r="J128" s="160" t="s">
+      <c r="J128" s="157" t="s">
         <v>1112</v>
       </c>
-      <c r="K128" s="161" t="s">
+      <c r="K128" s="181" t="s">
         <v>1113</v>
       </c>
-      <c r="L128" s="161" t="s">
+      <c r="L128" s="158" t="s">
         <v>1113</v>
       </c>
-      <c r="M128" s="161" t="s">
+      <c r="M128" s="158" t="s">
         <v>1114</v>
       </c>
-      <c r="N128" s="161" t="s">
+      <c r="N128" s="181" t="s">
         <v>1115</v>
       </c>
-      <c r="O128" s="161" t="s">
+      <c r="O128" s="158" t="s">
         <v>1115</v>
       </c>
-      <c r="P128" s="162" t="s">
+      <c r="P128" s="159" t="s">
         <v>1116</v>
       </c>
-      <c r="Q128" s="162" t="s">
+      <c r="Q128" s="159" t="s">
         <v>1117</v>
       </c>
-      <c r="R128" s="166" t="s">
+      <c r="R128" s="163" t="s">
         <v>1118</v>
       </c>
     </row>
@@ -12398,16 +12496,16 @@
       <c r="J129" s="27" t="s">
         <v>1123</v>
       </c>
-      <c r="K129" s="49" t="s">
+      <c r="K129" s="181" t="s">
         <v>1124</v>
       </c>
       <c r="L129" s="49" t="s">
         <v>1124</v>
       </c>
-      <c r="M129" s="122" t="s">
+      <c r="M129" s="121" t="s">
         <v>1125</v>
       </c>
-      <c r="N129" s="49" t="s">
+      <c r="N129" s="181" t="s">
         <v>1126</v>
       </c>
       <c r="O129" s="49" t="s">
@@ -12448,7 +12546,7 @@
       <c r="J130" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K130" s="49">
+      <c r="K130" s="181">
         <v>493</v>
       </c>
       <c r="L130" s="49">
@@ -12457,7 +12555,7 @@
       <c r="M130" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N130" s="49" t="s">
+      <c r="N130" s="181" t="s">
         <v>1134</v>
       </c>
       <c r="O130" s="49" t="s">
@@ -12494,7 +12592,7 @@
       <c r="J131" s="53" t="s">
         <v>1139</v>
       </c>
-      <c r="K131" s="54" t="s">
+      <c r="K131" s="184" t="s">
         <v>1140</v>
       </c>
       <c r="L131" s="54" t="s">
@@ -12503,10 +12601,10 @@
       <c r="M131" s="54" t="s">
         <v>1141</v>
       </c>
-      <c r="N131" s="134" t="s">
+      <c r="N131" s="206" t="s">
         <v>1142</v>
       </c>
-      <c r="O131" s="134" t="s">
+      <c r="O131" s="131" t="s">
         <v>1142</v>
       </c>
       <c r="P131" s="65" t="s">
@@ -12544,7 +12642,7 @@
       <c r="J132" s="27" t="s">
         <v>1151</v>
       </c>
-      <c r="K132" s="49" t="s">
+      <c r="K132" s="181" t="s">
         <v>1152</v>
       </c>
       <c r="L132" s="49" t="s">
@@ -12553,7 +12651,7 @@
       <c r="M132" s="49" t="s">
         <v>1153</v>
       </c>
-      <c r="N132" s="49" t="s">
+      <c r="N132" s="181" t="s">
         <v>1154</v>
       </c>
       <c r="O132" s="49" t="s">
@@ -12594,7 +12692,7 @@
       <c r="J133" s="27" t="s">
         <v>1163</v>
       </c>
-      <c r="K133" s="49" t="s">
+      <c r="K133" s="181" t="s">
         <v>1164</v>
       </c>
       <c r="L133" s="49" t="s">
@@ -12603,7 +12701,7 @@
       <c r="M133" s="49" t="s">
         <v>1165</v>
       </c>
-      <c r="N133" s="49" t="s">
+      <c r="N133" s="181" t="s">
         <v>1166</v>
       </c>
       <c r="O133" s="49" t="s">
@@ -12644,7 +12742,7 @@
       <c r="J134" s="27" t="s">
         <v>1174</v>
       </c>
-      <c r="K134" s="49">
+      <c r="K134" s="181">
         <v>571</v>
       </c>
       <c r="L134" s="49">
@@ -12653,7 +12751,7 @@
       <c r="M134" s="49" t="s">
         <v>1175</v>
       </c>
-      <c r="N134" s="49" t="s">
+      <c r="N134" s="181" t="s">
         <v>1176</v>
       </c>
       <c r="O134" s="49" t="s">
@@ -12694,7 +12792,7 @@
       <c r="J135" s="27" t="s">
         <v>1183</v>
       </c>
-      <c r="K135" s="49" t="s">
+      <c r="K135" s="181" t="s">
         <v>1184</v>
       </c>
       <c r="L135" s="49" t="s">
@@ -12703,7 +12801,7 @@
       <c r="M135" s="49" t="s">
         <v>1185</v>
       </c>
-      <c r="N135" s="49" t="s">
+      <c r="N135" s="181" t="s">
         <v>1186</v>
       </c>
       <c r="O135" s="49" t="s">
@@ -12721,7 +12819,7 @@
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A136" s="8"/>
-      <c r="B136" s="135">
+      <c r="B136" s="132">
         <v>1181</v>
       </c>
       <c r="C136" s="97"/>
@@ -12736,14 +12834,14 @@
       <c r="H136" s="99"/>
       <c r="I136" s="102"/>
       <c r="J136" s="102"/>
-      <c r="K136" s="103">
+      <c r="K136" s="181">
         <v>535</v>
       </c>
       <c r="L136" s="103">
         <v>535</v>
       </c>
       <c r="M136" s="103"/>
-      <c r="N136" s="103" t="s">
+      <c r="N136" s="181" t="s">
         <v>1189</v>
       </c>
       <c r="O136" s="103" t="s">
@@ -12755,7 +12853,7 @@
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A137" s="8"/>
-      <c r="B137" s="135">
+      <c r="B137" s="132">
         <v>1182</v>
       </c>
       <c r="C137" s="97"/>
@@ -12770,14 +12868,14 @@
       <c r="H137" s="99"/>
       <c r="I137" s="102"/>
       <c r="J137" s="102"/>
-      <c r="K137" s="103">
+      <c r="K137" s="181">
         <v>560</v>
       </c>
       <c r="L137" s="103">
         <v>560</v>
       </c>
       <c r="M137" s="103"/>
-      <c r="N137" s="103" t="s">
+      <c r="N137" s="181" t="s">
         <v>1191</v>
       </c>
       <c r="O137" s="103" t="s">
@@ -12789,7 +12887,7 @@
     </row>
     <row r="138" spans="1:18" ht="26" x14ac:dyDescent="0.2">
       <c r="A138" s="8"/>
-      <c r="B138" s="135">
+      <c r="B138" s="132">
         <v>1183</v>
       </c>
       <c r="C138" s="97"/>
@@ -12804,14 +12902,14 @@
       <c r="H138" s="99"/>
       <c r="I138" s="102"/>
       <c r="J138" s="102"/>
-      <c r="K138" s="136" t="s">
+      <c r="K138" s="199" t="s">
         <v>1193</v>
       </c>
-      <c r="L138" s="136" t="s">
+      <c r="L138" s="133" t="s">
         <v>1194</v>
       </c>
       <c r="M138" s="103"/>
-      <c r="N138" s="103" t="s">
+      <c r="N138" s="181" t="s">
         <v>1195</v>
       </c>
       <c r="O138" s="103" t="s">
@@ -12823,7 +12921,7 @@
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A139" s="8"/>
-      <c r="B139" s="135">
+      <c r="B139" s="132">
         <v>1184</v>
       </c>
       <c r="C139" s="97"/>
@@ -12838,14 +12936,14 @@
       <c r="H139" s="99"/>
       <c r="I139" s="102"/>
       <c r="J139" s="102"/>
-      <c r="K139" s="103" t="s">
+      <c r="K139" s="181" t="s">
         <v>1198</v>
       </c>
       <c r="L139" s="103" t="s">
         <v>1198</v>
       </c>
       <c r="M139" s="103"/>
-      <c r="N139" s="103" t="s">
+      <c r="N139" s="181" t="s">
         <v>1199</v>
       </c>
       <c r="O139" s="103" t="s">
@@ -12857,7 +12955,7 @@
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A140" s="8"/>
-      <c r="B140" s="135">
+      <c r="B140" s="132">
         <v>1185</v>
       </c>
       <c r="C140" s="97"/>
@@ -12872,14 +12970,14 @@
       <c r="H140" s="99"/>
       <c r="I140" s="102"/>
       <c r="J140" s="102"/>
-      <c r="K140" s="103" t="s">
+      <c r="K140" s="181" t="s">
         <v>1201</v>
       </c>
       <c r="L140" s="103">
         <v>577</v>
       </c>
       <c r="M140" s="103"/>
-      <c r="N140" s="103" t="s">
+      <c r="N140" s="181" t="s">
         <v>1202</v>
       </c>
       <c r="O140" s="103" t="s">
@@ -12893,7 +12991,7 @@
       <c r="A141" s="8" t="s">
         <v>1203</v>
       </c>
-      <c r="B141" s="137" t="s">
+      <c r="B141" s="134" t="s">
         <v>1204</v>
       </c>
       <c r="C141" s="52"/>
@@ -12912,7 +13010,7 @@
       <c r="J141" s="53" t="s">
         <v>1207</v>
       </c>
-      <c r="K141" s="54" t="s">
+      <c r="K141" s="184" t="s">
         <v>1208</v>
       </c>
       <c r="L141" s="54" t="s">
@@ -12921,7 +13019,7 @@
       <c r="M141" s="54" t="s">
         <v>1210</v>
       </c>
-      <c r="N141" s="54" t="s">
+      <c r="N141" s="184" t="s">
         <v>1211</v>
       </c>
       <c r="O141" s="54" t="s">
@@ -12937,53 +13035,53 @@
         <v>1215</v>
       </c>
     </row>
-    <row r="142" spans="1:18" s="163" customFormat="1" ht="39" x14ac:dyDescent="0.2">
-      <c r="A142" s="153" t="s">
+    <row r="142" spans="1:18" s="160" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A142" s="150" t="s">
         <v>1216</v>
       </c>
-      <c r="B142" s="154" t="s">
+      <c r="B142" s="151" t="s">
         <v>1217</v>
       </c>
-      <c r="C142" s="155" t="s">
+      <c r="C142" s="152" t="s">
         <v>1218</v>
       </c>
-      <c r="D142" s="156"/>
-      <c r="E142" s="157" t="s">
+      <c r="D142" s="153"/>
+      <c r="E142" s="154" t="s">
         <v>1219</v>
       </c>
-      <c r="F142" s="158" t="s">
+      <c r="F142" s="155" t="s">
         <v>1220</v>
       </c>
-      <c r="G142" s="159"/>
-      <c r="H142" s="159"/>
-      <c r="I142" s="160" t="s">
+      <c r="G142" s="156"/>
+      <c r="H142" s="156"/>
+      <c r="I142" s="157" t="s">
         <v>1221</v>
       </c>
-      <c r="J142" s="160" t="s">
+      <c r="J142" s="157" t="s">
         <v>1222</v>
       </c>
-      <c r="K142" s="161" t="s">
+      <c r="K142" s="181" t="s">
         <v>1223</v>
       </c>
-      <c r="L142" s="161" t="s">
+      <c r="L142" s="158" t="s">
         <v>1223</v>
       </c>
-      <c r="M142" s="161" t="s">
+      <c r="M142" s="158" t="s">
         <v>1224</v>
       </c>
-      <c r="N142" s="161" t="s">
+      <c r="N142" s="181" t="s">
         <v>1225</v>
       </c>
-      <c r="O142" s="161" t="s">
+      <c r="O142" s="158" t="s">
         <v>1225</v>
       </c>
-      <c r="P142" s="162" t="s">
+      <c r="P142" s="159" t="s">
         <v>1226</v>
       </c>
-      <c r="Q142" s="162" t="s">
+      <c r="Q142" s="159" t="s">
         <v>1227</v>
       </c>
-      <c r="R142" s="166" t="s">
+      <c r="R142" s="163" t="s">
         <v>1228</v>
       </c>
     </row>
@@ -12994,7 +13092,7 @@
       <c r="B143" s="9" t="s">
         <v>1230</v>
       </c>
-      <c r="C143" s="138" t="s">
+      <c r="C143" s="135" t="s">
         <v>1231</v>
       </c>
       <c r="D143" s="47"/>
@@ -13012,7 +13110,7 @@
       <c r="J143" s="27" t="s">
         <v>1234</v>
       </c>
-      <c r="K143" s="49" t="s">
+      <c r="K143" s="181" t="s">
         <v>1235</v>
       </c>
       <c r="L143" s="49" t="s">
@@ -13021,7 +13119,7 @@
       <c r="M143" s="49" t="s">
         <v>1236</v>
       </c>
-      <c r="N143" s="49" t="s">
+      <c r="N143" s="181" t="s">
         <v>1237</v>
       </c>
       <c r="O143" s="49" t="s">
@@ -13062,7 +13160,7 @@
       <c r="J144" s="27" t="s">
         <v>1244</v>
       </c>
-      <c r="K144" s="49">
+      <c r="K144" s="181">
         <v>600</v>
       </c>
       <c r="L144" s="49">
@@ -13071,7 +13169,7 @@
       <c r="M144" s="49" t="s">
         <v>1245</v>
       </c>
-      <c r="N144" s="49" t="s">
+      <c r="N144" s="181" t="s">
         <v>1246</v>
       </c>
       <c r="O144" s="49" t="s">
@@ -13108,7 +13206,7 @@
       <c r="J145" s="53" t="s">
         <v>1252</v>
       </c>
-      <c r="K145" s="54" t="s">
+      <c r="K145" s="184" t="s">
         <v>1253</v>
       </c>
       <c r="L145" s="54" t="s">
@@ -13117,7 +13215,7 @@
       <c r="M145" s="54" t="s">
         <v>1254</v>
       </c>
-      <c r="N145" s="54" t="s">
+      <c r="N145" s="184" t="s">
         <v>1255</v>
       </c>
       <c r="O145" s="54" t="s">
@@ -13158,7 +13256,7 @@
       <c r="J146" s="27" t="s">
         <v>1264</v>
       </c>
-      <c r="K146" s="49" t="s">
+      <c r="K146" s="181" t="s">
         <v>1265</v>
       </c>
       <c r="L146" s="49" t="s">
@@ -13167,7 +13265,7 @@
       <c r="M146" s="49" t="s">
         <v>1266</v>
       </c>
-      <c r="N146" s="49" t="s">
+      <c r="N146" s="181" t="s">
         <v>1267</v>
       </c>
       <c r="O146" s="49" t="s">
@@ -13208,7 +13306,7 @@
       <c r="J147" s="27" t="s">
         <v>1275</v>
       </c>
-      <c r="K147" s="49" t="s">
+      <c r="K147" s="181" t="s">
         <v>1276</v>
       </c>
       <c r="L147" s="49" t="s">
@@ -13217,7 +13315,7 @@
       <c r="M147" s="49" t="s">
         <v>1277</v>
       </c>
-      <c r="N147" s="49" t="s">
+      <c r="N147" s="181" t="s">
         <v>1278</v>
       </c>
       <c r="O147" s="49" t="s">
@@ -13258,7 +13356,7 @@
       <c r="J148" s="27" t="s">
         <v>1263</v>
       </c>
-      <c r="K148" s="49">
+      <c r="K148" s="181">
         <v>714</v>
       </c>
       <c r="L148" s="49">
@@ -13267,7 +13365,7 @@
       <c r="M148" s="49" t="s">
         <v>1286</v>
       </c>
-      <c r="N148" s="49" t="s">
+      <c r="N148" s="181" t="s">
         <v>1287</v>
       </c>
       <c r="O148" s="49" t="s">
@@ -13308,7 +13406,7 @@
       <c r="J149" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K149" s="49">
+      <c r="K149" s="181">
         <v>715</v>
       </c>
       <c r="L149" s="49">
@@ -13317,7 +13415,7 @@
       <c r="M149" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N149" s="49" t="s">
+      <c r="N149" s="181" t="s">
         <v>1292</v>
       </c>
       <c r="O149" s="49" t="s">
@@ -13343,7 +13441,7 @@
       <c r="C150" s="52"/>
       <c r="D150" s="60"/>
       <c r="E150" s="61"/>
-      <c r="F150" s="124" t="s">
+      <c r="F150" s="122" t="s">
         <v>107</v>
       </c>
       <c r="G150" s="95" t="s">
@@ -13356,7 +13454,7 @@
       <c r="J150" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K150" s="54">
+      <c r="K150" s="184">
         <v>274</v>
       </c>
       <c r="L150" s="54">
@@ -13365,7 +13463,7 @@
       <c r="M150" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N150" s="54" t="s">
+      <c r="N150" s="184" t="s">
         <v>1296</v>
       </c>
       <c r="O150" s="54" t="s">
@@ -13391,7 +13489,7 @@
       <c r="C151" s="52"/>
       <c r="D151" s="60"/>
       <c r="E151" s="61"/>
-      <c r="F151" s="124" t="s">
+      <c r="F151" s="122" t="s">
         <v>117</v>
       </c>
       <c r="G151" s="95" t="s">
@@ -13404,7 +13502,7 @@
       <c r="J151" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K151" s="78" t="s">
+      <c r="K151" s="186" t="s">
         <v>1300</v>
       </c>
       <c r="L151" s="78" t="s">
@@ -13413,7 +13511,7 @@
       <c r="M151" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N151" s="54" t="s">
+      <c r="N151" s="184" t="s">
         <v>1302</v>
       </c>
       <c r="O151" s="54" t="s">
@@ -13450,7 +13548,7 @@
       <c r="J152" s="53" t="s">
         <v>1308</v>
       </c>
-      <c r="K152" s="78" t="s">
+      <c r="K152" s="186" t="s">
         <v>1309</v>
       </c>
       <c r="L152" s="78" t="s">
@@ -13459,7 +13557,7 @@
       <c r="M152" s="54" t="s">
         <v>1311</v>
       </c>
-      <c r="N152" s="54" t="s">
+      <c r="N152" s="184" t="s">
         <v>1312</v>
       </c>
       <c r="O152" s="54" t="s">
@@ -13500,7 +13598,7 @@
       <c r="J153" s="27" t="s">
         <v>1320</v>
       </c>
-      <c r="K153" s="49" t="s">
+      <c r="K153" s="181" t="s">
         <v>1321</v>
       </c>
       <c r="L153" s="49" t="s">
@@ -13509,7 +13607,7 @@
       <c r="M153" s="49" t="s">
         <v>1322</v>
       </c>
-      <c r="N153" s="49" t="s">
+      <c r="N153" s="181" t="s">
         <v>1323</v>
       </c>
       <c r="O153" s="49" t="s">
@@ -13550,7 +13648,7 @@
       <c r="J154" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K154" s="122">
+      <c r="K154" s="200">
         <v>756.7</v>
       </c>
       <c r="L154" s="50" t="s">
@@ -13559,7 +13657,7 @@
       <c r="M154" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N154" s="122" t="s">
+      <c r="N154" s="200" t="s">
         <v>1330</v>
       </c>
       <c r="O154" s="50" t="s">
@@ -13600,7 +13698,7 @@
       <c r="J155" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K155" s="51" t="s">
+      <c r="K155" s="183" t="s">
         <v>1335</v>
       </c>
       <c r="L155" s="50" t="s">
@@ -13609,7 +13707,7 @@
       <c r="M155" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N155" s="49" t="s">
+      <c r="N155" s="181" t="s">
         <v>1336</v>
       </c>
       <c r="O155" s="49" t="s">
@@ -13650,7 +13748,7 @@
       <c r="J156" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K156" s="51" t="s">
+      <c r="K156" s="183" t="s">
         <v>1341</v>
       </c>
       <c r="L156" s="50" t="s">
@@ -13659,7 +13757,7 @@
       <c r="M156" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N156" s="49" t="s">
+      <c r="N156" s="181" t="s">
         <v>1342</v>
       </c>
       <c r="O156" s="49" t="s">
@@ -13700,7 +13798,7 @@
       <c r="J157" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K157" s="51" t="s">
+      <c r="K157" s="183" t="s">
         <v>1347</v>
       </c>
       <c r="L157" s="50" t="s">
@@ -13709,7 +13807,7 @@
       <c r="M157" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N157" s="49" t="s">
+      <c r="N157" s="181" t="s">
         <v>1348</v>
       </c>
       <c r="O157" s="49" t="s">
@@ -13750,7 +13848,7 @@
       <c r="J158" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K158" s="51" t="s">
+      <c r="K158" s="183" t="s">
         <v>1353</v>
       </c>
       <c r="L158" s="50" t="s">
@@ -13759,7 +13857,7 @@
       <c r="M158" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N158" s="49" t="s">
+      <c r="N158" s="181" t="s">
         <v>1354</v>
       </c>
       <c r="O158" s="49" t="s">
@@ -13800,7 +13898,7 @@
       <c r="J159" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K159" s="49">
+      <c r="K159" s="181">
         <v>750.3</v>
       </c>
       <c r="L159" s="50" t="s">
@@ -13809,7 +13907,7 @@
       <c r="M159" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N159" s="49" t="s">
+      <c r="N159" s="181" t="s">
         <v>1359</v>
       </c>
       <c r="O159" s="50" t="s">
@@ -13850,7 +13948,7 @@
       <c r="J160" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K160" s="51" t="s">
+      <c r="K160" s="183" t="s">
         <v>1364</v>
       </c>
       <c r="L160" s="50" t="s">
@@ -13859,7 +13957,7 @@
       <c r="M160" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N160" s="49" t="s">
+      <c r="N160" s="181" t="s">
         <v>1365</v>
       </c>
       <c r="O160" s="49" t="s">
@@ -13900,7 +13998,7 @@
       <c r="J161" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K161" s="51" t="s">
+      <c r="K161" s="183" t="s">
         <v>1370</v>
       </c>
       <c r="L161" s="50" t="s">
@@ -13909,7 +14007,7 @@
       <c r="M161" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N161" s="49" t="s">
+      <c r="N161" s="181" t="s">
         <v>1371</v>
       </c>
       <c r="O161" s="49" t="s">
@@ -13950,7 +14048,7 @@
       <c r="J162" s="27" t="s">
         <v>1376</v>
       </c>
-      <c r="K162" s="49" t="s">
+      <c r="K162" s="181" t="s">
         <v>1377</v>
       </c>
       <c r="L162" s="49" t="s">
@@ -13959,7 +14057,7 @@
       <c r="M162" s="49" t="s">
         <v>1378</v>
       </c>
-      <c r="N162" s="49" t="s">
+      <c r="N162" s="181" t="s">
         <v>1379</v>
       </c>
       <c r="O162" s="49" t="s">
@@ -14000,7 +14098,7 @@
       <c r="J163" s="27" t="s">
         <v>1385</v>
       </c>
-      <c r="K163" s="49">
+      <c r="K163" s="181">
         <v>741</v>
       </c>
       <c r="L163" s="49">
@@ -14009,7 +14107,7 @@
       <c r="M163" s="49" t="s">
         <v>1386</v>
       </c>
-      <c r="N163" s="49" t="s">
+      <c r="N163" s="181" t="s">
         <v>1387</v>
       </c>
       <c r="O163" s="49" t="s">
@@ -14035,7 +14133,7 @@
       <c r="C164" s="52"/>
       <c r="D164" s="60"/>
       <c r="E164" s="61"/>
-      <c r="G164" s="139" t="s">
+      <c r="G164" s="136" t="s">
         <v>1390</v>
       </c>
       <c r="H164" s="52"/>
@@ -14045,7 +14143,7 @@
       <c r="J164" s="53" t="s">
         <v>1392</v>
       </c>
-      <c r="K164" s="54" t="s">
+      <c r="K164" s="184" t="s">
         <v>1393</v>
       </c>
       <c r="L164" s="54" t="s">
@@ -14054,7 +14152,7 @@
       <c r="M164" s="54" t="s">
         <v>1395</v>
       </c>
-      <c r="N164" s="54" t="s">
+      <c r="N164" s="184" t="s">
         <v>1396</v>
       </c>
       <c r="O164" s="54" t="s">
@@ -14095,7 +14193,7 @@
       <c r="J165" s="27" t="s">
         <v>1405</v>
       </c>
-      <c r="K165" s="49" t="s">
+      <c r="K165" s="181" t="s">
         <v>1406</v>
       </c>
       <c r="L165" s="49" t="s">
@@ -14104,7 +14202,7 @@
       <c r="M165" s="49" t="s">
         <v>1407</v>
       </c>
-      <c r="N165" s="49" t="s">
+      <c r="N165" s="181" t="s">
         <v>1408</v>
       </c>
       <c r="O165" s="49" t="s">
@@ -14145,7 +14243,7 @@
       <c r="J166" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K166" s="51" t="s">
+      <c r="K166" s="183" t="s">
         <v>1413</v>
       </c>
       <c r="L166" s="50" t="s">
@@ -14154,7 +14252,7 @@
       <c r="M166" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N166" s="49" t="s">
+      <c r="N166" s="181" t="s">
         <v>1414</v>
       </c>
       <c r="O166" s="49" t="s">
@@ -14195,7 +14293,7 @@
       <c r="J167" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K167" s="49">
+      <c r="K167" s="181">
         <v>523</v>
       </c>
       <c r="L167" s="49">
@@ -14204,7 +14302,7 @@
       <c r="M167" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N167" s="49" t="s">
+      <c r="N167" s="181" t="s">
         <v>1419</v>
       </c>
       <c r="O167" s="49" t="s">
@@ -14245,7 +14343,7 @@
       <c r="J168" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K168" s="50" t="s">
+      <c r="K168" s="182" t="s">
         <v>69</v>
       </c>
       <c r="L168" s="50" t="s">
@@ -14254,7 +14352,7 @@
       <c r="M168" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N168" s="27" t="s">
+      <c r="N168" s="185" t="s">
         <v>69</v>
       </c>
       <c r="O168" s="27" t="s">
@@ -14281,7 +14379,7 @@
       <c r="D169" s="60"/>
       <c r="E169" s="61"/>
       <c r="F169" s="70"/>
-      <c r="G169" s="139" t="s">
+      <c r="G169" s="136" t="s">
         <v>1426</v>
       </c>
       <c r="H169" s="52"/>
@@ -14291,7 +14389,7 @@
       <c r="J169" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K169" s="54" t="s">
+      <c r="K169" s="184" t="s">
         <v>1427</v>
       </c>
       <c r="L169" s="54" t="s">
@@ -14300,7 +14398,7 @@
       <c r="M169" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="N169" s="54" t="s">
+      <c r="N169" s="184" t="s">
         <v>1429</v>
       </c>
       <c r="O169" s="54" t="s">
@@ -14318,32 +14416,32 @@
     </row>
     <row r="170" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A170" s="8"/>
-      <c r="B170" s="135">
+      <c r="B170" s="132">
         <v>1475</v>
       </c>
-      <c r="C170" s="140"/>
+      <c r="C170" s="137"/>
       <c r="D170" s="98"/>
       <c r="E170" s="99" t="s">
         <v>1430</v>
       </c>
-      <c r="F170" s="141" t="s">
+      <c r="F170" s="138" t="s">
         <v>1431</v>
       </c>
-      <c r="G170" s="142"/>
-      <c r="H170" s="142"/>
+      <c r="G170" s="139"/>
+      <c r="H170" s="139"/>
       <c r="I170" s="102"/>
       <c r="J170" s="102"/>
-      <c r="K170" s="99">
+      <c r="K170" s="201">
         <v>7980</v>
       </c>
-      <c r="L170" s="143"/>
+      <c r="L170" s="140"/>
       <c r="M170" s="105" t="s">
         <v>1432</v>
       </c>
-      <c r="N170" s="144" t="s">
+      <c r="N170" s="207" t="s">
         <v>1433</v>
       </c>
-      <c r="O170" s="144" t="s">
+      <c r="O170" s="141" t="s">
         <v>1433</v>
       </c>
       <c r="P170" s="105"/>
@@ -14351,7 +14449,7 @@
       <c r="R170" s="105"/>
     </row>
     <row r="171" spans="1:18" ht="39" x14ac:dyDescent="0.2">
-      <c r="A171" s="145" t="s">
+      <c r="A171" s="142" t="s">
         <v>1434</v>
       </c>
       <c r="B171" s="9" t="s">
@@ -14360,22 +14458,22 @@
       <c r="C171" s="44" t="s">
         <v>1436</v>
       </c>
-      <c r="D171" s="146" t="s">
+      <c r="D171" s="143" t="s">
         <v>1437</v>
       </c>
-      <c r="E171" s="147" t="s">
+      <c r="E171" s="144" t="s">
         <v>1438</v>
       </c>
-      <c r="F171" s="148"/>
-      <c r="G171" s="148"/>
-      <c r="H171" s="148"/>
+      <c r="F171" s="145"/>
+      <c r="G171" s="145"/>
+      <c r="H171" s="145"/>
       <c r="I171" s="27" t="s">
         <v>1439</v>
       </c>
       <c r="J171" s="27" t="s">
         <v>1439</v>
       </c>
-      <c r="K171" s="49" t="s">
+      <c r="K171" s="181" t="s">
         <v>1440</v>
       </c>
       <c r="L171" s="49" t="s">
@@ -14384,7 +14482,7 @@
       <c r="M171" s="49" t="s">
         <v>1441</v>
       </c>
-      <c r="N171" s="49" t="s">
+      <c r="N171" s="181" t="s">
         <v>1442</v>
       </c>
       <c r="O171" s="49" t="s">
@@ -14425,7 +14523,7 @@
       <c r="J172" s="27" t="s">
         <v>1451</v>
       </c>
-      <c r="K172" s="49" t="s">
+      <c r="K172" s="181" t="s">
         <v>1452</v>
       </c>
       <c r="L172" s="49" t="s">
@@ -14434,7 +14532,7 @@
       <c r="M172" s="49" t="s">
         <v>1453</v>
       </c>
-      <c r="N172" s="49" t="s">
+      <c r="N172" s="181" t="s">
         <v>1454</v>
       </c>
       <c r="O172" s="49" t="s">
@@ -14468,14 +14566,14 @@
       <c r="G173" s="95" t="s">
         <v>1461</v>
       </c>
-      <c r="H173" s="149"/>
+      <c r="H173" s="146"/>
       <c r="I173" s="27" t="s">
         <v>1462</v>
       </c>
       <c r="J173" s="27" t="s">
         <v>1462</v>
       </c>
-      <c r="K173" s="49" t="s">
+      <c r="K173" s="181" t="s">
         <v>1463</v>
       </c>
       <c r="L173" s="49" t="s">
@@ -14484,10 +14582,10 @@
       <c r="M173" s="49" t="s">
         <v>1465</v>
       </c>
-      <c r="N173" s="150" t="s">
+      <c r="N173" s="207" t="s">
         <v>1466</v>
       </c>
-      <c r="O173" s="150" t="s">
+      <c r="O173" s="147" t="s">
         <v>1466</v>
       </c>
       <c r="P173" s="49" t="s">
@@ -14525,7 +14623,7 @@
       <c r="J174" s="27" t="s">
         <v>1474</v>
       </c>
-      <c r="K174" s="49" t="s">
+      <c r="K174" s="181" t="s">
         <v>1475</v>
       </c>
       <c r="L174" s="49" t="s">
@@ -14534,7 +14632,7 @@
       <c r="M174" s="49" t="s">
         <v>1476</v>
       </c>
-      <c r="N174" s="49" t="s">
+      <c r="N174" s="181" t="s">
         <v>1477</v>
       </c>
       <c r="O174" s="49" t="s">
@@ -14575,7 +14673,7 @@
       <c r="J175" s="27" t="s">
         <v>1484</v>
       </c>
-      <c r="K175" s="49" t="s">
+      <c r="K175" s="181" t="s">
         <v>1485</v>
       </c>
       <c r="L175" s="49" t="s">
@@ -14584,7 +14682,7 @@
       <c r="M175" s="49" t="s">
         <v>1486</v>
       </c>
-      <c r="N175" s="49" t="s">
+      <c r="N175" s="181" t="s">
         <v>1487</v>
       </c>
       <c r="O175" s="49" t="s">
@@ -14625,7 +14723,7 @@
       <c r="J176" s="27" t="s">
         <v>1495</v>
       </c>
-      <c r="K176" s="49" t="s">
+      <c r="K176" s="181" t="s">
         <v>1496</v>
       </c>
       <c r="L176" s="49" t="s">
@@ -14634,7 +14732,7 @@
       <c r="M176" s="49" t="s">
         <v>1497</v>
       </c>
-      <c r="N176" s="49" t="s">
+      <c r="N176" s="181" t="s">
         <v>1498</v>
       </c>
       <c r="O176" s="49" t="s">
@@ -14675,7 +14773,7 @@
       <c r="J177" s="27" t="s">
         <v>1494</v>
       </c>
-      <c r="K177" s="49" t="s">
+      <c r="K177" s="181" t="s">
         <v>1506</v>
       </c>
       <c r="L177" s="49" t="s">
@@ -14684,7 +14782,7 @@
       <c r="M177" s="49" t="s">
         <v>1507</v>
       </c>
-      <c r="N177" s="49" t="s">
+      <c r="N177" s="181" t="s">
         <v>1508</v>
       </c>
       <c r="O177" s="49" t="s">
@@ -14702,7 +14800,7 @@
     </row>
     <row r="178" spans="1:18" ht="65" x14ac:dyDescent="0.2">
       <c r="A178" s="8"/>
-      <c r="B178" s="135">
+      <c r="B178" s="132">
         <v>1541</v>
       </c>
       <c r="C178" s="97"/>
@@ -14717,14 +14815,14 @@
       <c r="H178" s="99"/>
       <c r="I178" s="102"/>
       <c r="J178" s="102"/>
-      <c r="K178" s="103" t="s">
+      <c r="K178" s="181" t="s">
         <v>1513</v>
       </c>
       <c r="L178" s="103" t="s">
         <v>1514</v>
       </c>
       <c r="M178" s="103"/>
-      <c r="N178" s="103" t="s">
+      <c r="N178" s="181" t="s">
         <v>1515</v>
       </c>
       <c r="O178" s="103" t="s">
@@ -14736,7 +14834,7 @@
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A179" s="8"/>
-      <c r="B179" s="135">
+      <c r="B179" s="132">
         <v>1542</v>
       </c>
       <c r="C179" s="97"/>
@@ -14751,7 +14849,7 @@
       <c r="H179" s="99"/>
       <c r="I179" s="102"/>
       <c r="J179" s="102"/>
-      <c r="K179" s="103" t="s">
+      <c r="K179" s="181" t="s">
         <v>1517</v>
       </c>
       <c r="L179" s="103" t="s">
@@ -14760,7 +14858,7 @@
       <c r="M179" s="103" t="s">
         <v>1518</v>
       </c>
-      <c r="N179" s="103" t="s">
+      <c r="N179" s="181" t="s">
         <v>1519</v>
       </c>
       <c r="O179" s="103" t="s">
@@ -14781,8 +14879,8 @@
         <v>1522</v>
       </c>
       <c r="D180" s="60"/>
-      <c r="E180" s="151"/>
-      <c r="F180" s="124" t="s">
+      <c r="E180" s="148"/>
+      <c r="F180" s="122" t="s">
         <v>231</v>
       </c>
       <c r="G180" s="95" t="s">
@@ -14795,7 +14893,7 @@
       <c r="J180" s="53" t="s">
         <v>1525</v>
       </c>
-      <c r="K180" s="54" t="s">
+      <c r="K180" s="184" t="s">
         <v>1526</v>
       </c>
       <c r="L180" s="54" t="s">
@@ -14804,10 +14902,10 @@
       <c r="M180" s="54" t="s">
         <v>1528</v>
       </c>
-      <c r="N180" s="152" t="s">
+      <c r="N180" s="208" t="s">
         <v>1529</v>
       </c>
-      <c r="O180" s="152" t="s">
+      <c r="O180" s="149" t="s">
         <v>1530</v>
       </c>
       <c r="P180" s="65" t="s">
@@ -14845,7 +14943,7 @@
       <c r="J181" s="27" t="s">
         <v>1539</v>
       </c>
-      <c r="K181" s="49" t="s">
+      <c r="K181" s="181" t="s">
         <v>1540</v>
       </c>
       <c r="L181" s="49" t="s">
@@ -14854,7 +14952,7 @@
       <c r="M181" s="49" t="s">
         <v>1541</v>
       </c>
-      <c r="N181" s="49" t="s">
+      <c r="N181" s="181" t="s">
         <v>1542</v>
       </c>
       <c r="O181" s="49" t="s">
@@ -14895,7 +14993,7 @@
       <c r="J182" s="27" t="s">
         <v>1552</v>
       </c>
-      <c r="K182" s="49" t="s">
+      <c r="K182" s="181" t="s">
         <v>1553</v>
       </c>
       <c r="L182" s="49" t="s">
@@ -14904,7 +15002,7 @@
       <c r="M182" s="49" t="s">
         <v>1554</v>
       </c>
-      <c r="N182" s="49" t="s">
+      <c r="N182" s="181" t="s">
         <v>1555</v>
       </c>
       <c r="O182" s="49" t="s">
@@ -14938,14 +15036,14 @@
       <c r="G183" s="95" t="s">
         <v>1562</v>
       </c>
-      <c r="H183" s="149"/>
+      <c r="H183" s="146"/>
       <c r="I183" s="27" t="s">
         <v>1563</v>
       </c>
       <c r="J183" s="27" t="s">
         <v>1551</v>
       </c>
-      <c r="K183" s="49" t="s">
+      <c r="K183" s="181" t="s">
         <v>1564</v>
       </c>
       <c r="L183" s="49" t="s">
@@ -14954,7 +15052,7 @@
       <c r="M183" s="49" t="s">
         <v>281</v>
       </c>
-      <c r="N183" s="49" t="s">
+      <c r="N183" s="181" t="s">
         <v>1565</v>
       </c>
       <c r="O183" s="49" t="s">
@@ -14995,7 +15093,7 @@
       <c r="J184" s="27" t="s">
         <v>1573</v>
       </c>
-      <c r="K184" s="49" t="s">
+      <c r="K184" s="181" t="s">
         <v>1574</v>
       </c>
       <c r="L184" s="49" t="s">
@@ -15004,7 +15102,7 @@
       <c r="M184" s="49" t="s">
         <v>1575</v>
       </c>
-      <c r="N184" s="49" t="s">
+      <c r="N184" s="181" t="s">
         <v>1576</v>
       </c>
       <c r="O184" s="49" t="s">
@@ -15037,7 +15135,7 @@
       <c r="J185" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K185" s="54" t="s">
+      <c r="K185" s="184" t="s">
         <v>1580</v>
       </c>
       <c r="L185" s="54" t="s">
@@ -15046,7 +15144,7 @@
       <c r="M185" s="54" t="s">
         <v>1581</v>
       </c>
-      <c r="N185" s="54" t="s">
+      <c r="N185" s="184" t="s">
         <v>1582</v>
       </c>
       <c r="O185" s="54" t="s">

</xml_diff>